<commit_message>
add code of BBPSO & update PSO data
</commit_message>
<xml_diff>
--- a/萝卜代码开会/PSOs+测试函数+仿真结果/PSO.xlsx
+++ b/萝卜代码开会/PSOs+测试函数+仿真结果/PSO.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC50C37-BE61-4813-8735-8608E5C5936F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001338E2-62B2-453F-892C-2E8972768374}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
   <si>
     <t>基本PSO+Ackley</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,30 @@
   </si>
   <si>
     <t>breed-PSO+SDP</t>
+  </si>
+  <si>
+    <t>BBPSO+Ackley</t>
+  </si>
+  <si>
+    <t>BBPSO+Rastrigin</t>
+  </si>
+  <si>
+    <t>BBPSO+Griewank</t>
+  </si>
+  <si>
+    <t>BBPSO+Alpine</t>
+  </si>
+  <si>
+    <t>BBPSO+Sphere</t>
+  </si>
+  <si>
+    <t>BBPSO+Rosenbrock</t>
+  </si>
+  <si>
+    <t>BBPSO+Schwefel</t>
+  </si>
+  <si>
+    <t>BBPSO+SDP</t>
   </si>
 </sst>
 </file>
@@ -518,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB90"/>
+  <dimension ref="A1:BB108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="AM89" workbookViewId="0">
+      <selection activeCell="AX105" sqref="AX105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10400,11 +10424,11 @@
         <v>1.13028885427138</v>
       </c>
       <c r="BA67" s="1">
-        <f t="shared" ref="BA67:BA90" si="2">AVERAGE(C67:AZ67)</f>
+        <f t="shared" ref="BA67:BA108" si="2">AVERAGE(C67:AZ67)</f>
         <v>1.3061262637510567</v>
       </c>
       <c r="BB67" s="1">
-        <f t="shared" ref="BB67:BB90" si="3">STDEVP(C67:AZ67)</f>
+        <f t="shared" ref="BB67:BB108" si="3">STDEVP(C67:AZ67)</f>
         <v>0.13151924759816777</v>
       </c>
     </row>
@@ -13864,18 +13888,2706 @@
         <v>5.2374642067385681E-11</v>
       </c>
     </row>
+    <row r="91" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="BA91" s="1"/>
+      <c r="BB91" s="1"/>
+    </row>
+    <row r="92" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" t="s">
+        <v>48</v>
+      </c>
+      <c r="C92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="D92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="E92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="F92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="G92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="H92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="I92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="J92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="K92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="L92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="M92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="N92" s="1">
+        <v>1.6462236331031099</v>
+      </c>
+      <c r="O92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="P92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="Q92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="R92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="S92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="T92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="U92" s="1">
+        <v>19.934735103650102</v>
+      </c>
+      <c r="V92" s="1">
+        <v>1.6462236331031099</v>
+      </c>
+      <c r="W92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="X92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="Y92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="Z92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="AA92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AB92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AC92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AD92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AE92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AF92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="AG92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AH92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AI92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AJ92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AK92" s="1">
+        <v>1.1551485027098201</v>
+      </c>
+      <c r="AL92" s="1">
+        <v>2.01331523625579</v>
+      </c>
+      <c r="AM92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AN92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AO92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AP92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="AQ92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AR92" s="1">
+        <v>1.4210854715202001E-14</v>
+      </c>
+      <c r="AS92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AT92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AU92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AV92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AW92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="AX92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="AY92" s="1">
+        <v>7.1054273576010003E-15</v>
+      </c>
+      <c r="AZ92" s="1">
+        <v>3.5527136788005001E-15</v>
+      </c>
+      <c r="BA92" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5279129221764427</v>
+      </c>
+      <c r="BB92" s="1">
+        <f t="shared" si="3"/>
+        <v>2.8080846560845809</v>
+      </c>
+    </row>
+    <row r="93" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A93" s="2"/>
+      <c r="B93" t="s">
+        <v>49</v>
+      </c>
+      <c r="C93" s="1">
+        <v>13.9294116858488</v>
+      </c>
+      <c r="D93" s="1">
+        <v>7.9596674189272498</v>
+      </c>
+      <c r="E93" s="1">
+        <v>9.9495804952947502</v>
+      </c>
+      <c r="F93" s="1">
+        <v>5.9697493047406702</v>
+      </c>
+      <c r="G93" s="1">
+        <v>1.98991811418658</v>
+      </c>
+      <c r="H93" s="1">
+        <v>1.98991811418658</v>
+      </c>
+      <c r="I93" s="1">
+        <v>7.9596674189272498</v>
+      </c>
+      <c r="J93" s="1">
+        <v>9.9495855331138294</v>
+      </c>
+      <c r="K93" s="1">
+        <v>10.944539552387999</v>
+      </c>
+      <c r="L93" s="1">
+        <v>13.9294116858488</v>
+      </c>
+      <c r="M93" s="1">
+        <v>6.96470836183396</v>
+      </c>
+      <c r="N93" s="1">
+        <v>14.9243707429421</v>
+      </c>
+      <c r="O93" s="1">
+        <v>8.9546264760205396</v>
+      </c>
+      <c r="P93" s="1">
+        <v>9.9495804952947502</v>
+      </c>
+      <c r="Q93" s="1">
+        <v>8.9546264760205396</v>
+      </c>
+      <c r="R93" s="1">
+        <v>15.919309603321</v>
+      </c>
+      <c r="S93" s="1">
+        <v>7.9596674189272498</v>
+      </c>
+      <c r="T93" s="1">
+        <v>11.9394986094813</v>
+      </c>
+      <c r="U93" s="1">
+        <v>4.9747952854664499</v>
+      </c>
+      <c r="V93" s="1">
+        <v>12.9344576665746</v>
+      </c>
+      <c r="W93" s="1">
+        <v>19.899140793875102</v>
+      </c>
+      <c r="X93" s="1">
+        <v>10.944539552387999</v>
+      </c>
+      <c r="Y93" s="1">
+        <v>10.9445445902071</v>
+      </c>
+      <c r="Z93" s="1">
+        <v>15.919309603321</v>
+      </c>
+      <c r="AA93" s="1">
+        <v>11.9394986094813</v>
+      </c>
+      <c r="AB93" s="1">
+        <v>9.9495602985803</v>
+      </c>
+      <c r="AC93" s="1">
+        <v>1.98991811418658</v>
+      </c>
+      <c r="AD93" s="1">
+        <v>2.9848771712798698</v>
+      </c>
+      <c r="AE93" s="1">
+        <v>6.96470836183396</v>
+      </c>
+      <c r="AF93" s="1">
+        <v>5.9697493047406702</v>
+      </c>
+      <c r="AG93" s="1">
+        <v>9.9495804952947502</v>
+      </c>
+      <c r="AH93" s="1">
+        <v>6.9647133996530401</v>
+      </c>
+      <c r="AI93" s="1">
+        <v>7.9596674189272498</v>
+      </c>
+      <c r="AJ93" s="1">
+        <v>5.9697543425597397</v>
+      </c>
+      <c r="AK93" s="1">
+        <v>0.99495905709329002</v>
+      </c>
+      <c r="AL93" s="1">
+        <v>10.944539552387999</v>
+      </c>
+      <c r="AM93" s="1">
+        <v>7.9596674189272498</v>
+      </c>
+      <c r="AN93" s="1">
+        <v>6.96470836183396</v>
+      </c>
+      <c r="AO93" s="1">
+        <v>5.9697493047406702</v>
+      </c>
+      <c r="AP93" s="1">
+        <v>15.919329800035401</v>
+      </c>
+      <c r="AQ93" s="1">
+        <v>7.9596674189272498</v>
+      </c>
+      <c r="AR93" s="1">
+        <v>5.9697543425597397</v>
+      </c>
+      <c r="AS93" s="1">
+        <v>7.9596674189272498</v>
+      </c>
+      <c r="AT93" s="1">
+        <v>4.9747952854664499</v>
+      </c>
+      <c r="AU93" s="1">
+        <v>5.9697493047406702</v>
+      </c>
+      <c r="AV93" s="1">
+        <v>4.9747952854664499</v>
+      </c>
+      <c r="AW93" s="1">
+        <v>9.9495804952947502</v>
+      </c>
+      <c r="AX93" s="1">
+        <v>10.944539552387999</v>
+      </c>
+      <c r="AY93" s="1">
+        <v>5.9697543425597503</v>
+      </c>
+      <c r="AZ93" s="1">
+        <v>6.96470836183396</v>
+      </c>
+      <c r="BA93" s="1">
+        <f t="shared" si="2"/>
+        <v>8.735732356377131</v>
+      </c>
+      <c r="BB93" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9713126679372466</v>
+      </c>
+    </row>
+    <row r="94" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A94" s="2"/>
+      <c r="B94" t="s">
+        <v>50</v>
+      </c>
+      <c r="C94" s="1">
+        <v>8.6244538392177897E-2</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1.47797767548257E-2</v>
+      </c>
+      <c r="E94" s="1">
+        <v>3.4447721035204201E-2</v>
+      </c>
+      <c r="F94" s="1">
+        <v>0.11069008604656</v>
+      </c>
+      <c r="G94" s="1">
+        <v>5.8993969753774501E-2</v>
+      </c>
+      <c r="H94" s="1">
+        <v>3.9367751902749902E-2</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0.113131771065489</v>
+      </c>
+      <c r="J94" s="1">
+        <v>8.5962555850082098E-2</v>
+      </c>
+      <c r="K94" s="1">
+        <v>0.10327933447518001</v>
+      </c>
+      <c r="L94" s="1">
+        <v>5.6532793852475997E-2</v>
+      </c>
+      <c r="M94" s="1">
+        <v>3.4477131738378297E-2</v>
+      </c>
+      <c r="N94" s="1">
+        <v>0.20927274244483701</v>
+      </c>
+      <c r="O94" s="1">
+        <v>0.125523924945353</v>
+      </c>
+      <c r="P94" s="1">
+        <v>0.105745576539331</v>
+      </c>
+      <c r="Q94" s="1">
+        <v>0.110685205356093</v>
+      </c>
+      <c r="R94" s="1">
+        <v>3.6872127426345998E-2</v>
+      </c>
+      <c r="S94" s="1">
+        <v>9.1096063294929502E-2</v>
+      </c>
+      <c r="T94" s="1">
+        <v>0.110726869147735</v>
+      </c>
+      <c r="U94" s="1">
+        <v>0.113085113526057</v>
+      </c>
+      <c r="V94" s="1">
+        <v>7.3884205094477601E-2</v>
+      </c>
+      <c r="W94" s="1">
+        <v>0.110714705341194</v>
+      </c>
+      <c r="X94" s="1">
+        <v>0.103293999231846</v>
+      </c>
+      <c r="Y94" s="1">
+        <v>9.8408254187071401E-2</v>
+      </c>
+      <c r="Z94" s="1">
+        <v>5.4157348540295601E-2</v>
+      </c>
+      <c r="AA94" s="1">
+        <v>0.110641038985393</v>
+      </c>
+      <c r="AB94" s="1">
+        <v>6.8863587937716103E-2</v>
+      </c>
+      <c r="AC94" s="1">
+        <v>6.15804145812806E-2</v>
+      </c>
+      <c r="AD94" s="1">
+        <v>0.28061949800654301</v>
+      </c>
+      <c r="AE94" s="1">
+        <v>0.152575423900185</v>
+      </c>
+      <c r="AF94" s="1">
+        <v>1.7236111917661501E-2</v>
+      </c>
+      <c r="AG94" s="1">
+        <v>0.16000854912297599</v>
+      </c>
+      <c r="AH94" s="1">
+        <v>6.3948427670147398E-2</v>
+      </c>
+      <c r="AI94" s="1">
+        <v>2.7017420107750299E-2</v>
+      </c>
+      <c r="AJ94" s="1">
+        <v>0.10816751092157199</v>
+      </c>
+      <c r="AK94" s="1">
+        <v>9.5882481917776402E-2</v>
+      </c>
+      <c r="AL94" s="1">
+        <v>7.6225200922031694E-2</v>
+      </c>
+      <c r="AM94" s="1">
+        <v>6.1509183380916599E-2</v>
+      </c>
+      <c r="AN94" s="1">
+        <v>3.4467313380248797E-2</v>
+      </c>
+      <c r="AO94" s="1">
+        <v>6.6377702181141807E-2</v>
+      </c>
+      <c r="AP94" s="1">
+        <v>8.6205262487754494E-2</v>
+      </c>
+      <c r="AQ94" s="1">
+        <v>4.4258437230621603E-2</v>
+      </c>
+      <c r="AR94" s="1">
+        <v>0.103281832468036</v>
+      </c>
+      <c r="AS94" s="1">
+        <v>6.6419400940028406E-2</v>
+      </c>
+      <c r="AT94" s="1">
+        <v>0.14263234419530799</v>
+      </c>
+      <c r="AU94" s="1">
+        <v>6.6434107933606296E-2</v>
+      </c>
+      <c r="AV94" s="1">
+        <v>8.6075197168378997E-2</v>
+      </c>
+      <c r="AW94" s="1">
+        <v>3.69605095580278E-2</v>
+      </c>
+      <c r="AX94" s="1">
+        <v>8.6200360332355799E-2</v>
+      </c>
+      <c r="AY94" s="1">
+        <v>4.1838791941891003E-2</v>
+      </c>
+      <c r="AZ94" s="1">
+        <v>8.3662892757032203E-2</v>
+      </c>
+      <c r="BA94" s="1">
+        <f t="shared" si="2"/>
+        <v>8.6209251357776878E-2</v>
+      </c>
+      <c r="BB94" s="1">
+        <f t="shared" si="3"/>
+        <v>4.73799461019596E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A95" s="2"/>
+      <c r="B95" t="s">
+        <v>51</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2.72698530423554E-15</v>
+      </c>
+      <c r="D95" s="1">
+        <v>6.5503158452884196E-15</v>
+      </c>
+      <c r="E95" s="1">
+        <v>2.1094237467878002E-15</v>
+      </c>
+      <c r="F95" s="1">
+        <v>3.21964677141295E-15</v>
+      </c>
+      <c r="G95" s="1">
+        <v>7.2164496600635207E-15</v>
+      </c>
+      <c r="H95" s="1">
+        <v>4.3187675657918602E-14</v>
+      </c>
+      <c r="I95" s="1">
+        <v>6.6058269965196798E-15</v>
+      </c>
+      <c r="J95" s="1">
+        <v>2.5368596112684799E-14</v>
+      </c>
+      <c r="K95" s="1">
+        <v>8.8262730457699898E-15</v>
+      </c>
+      <c r="L95" s="1">
+        <v>7.8825834748386099E-15</v>
+      </c>
+      <c r="M95" s="1">
+        <v>5.1070259132757201E-15</v>
+      </c>
+      <c r="N95" s="1">
+        <v>1.6653345369377301E-15</v>
+      </c>
+      <c r="O95" s="1">
+        <v>3.8857805861880503E-15</v>
+      </c>
+      <c r="P95" s="1">
+        <v>4.0523140398818198E-15</v>
+      </c>
+      <c r="Q95" s="1">
+        <v>4.4408920985006301E-16</v>
+      </c>
+      <c r="R95" s="1">
+        <v>4.4408920985006301E-16</v>
+      </c>
+      <c r="S95" s="1">
+        <v>2.2593038551121901E-14</v>
+      </c>
+      <c r="T95" s="1">
+        <v>1.8651746813702601E-14</v>
+      </c>
+      <c r="U95" s="1">
+        <v>3.6637359812630197E-15</v>
+      </c>
+      <c r="V95" s="1">
+        <v>1.5543122344752199E-15</v>
+      </c>
+      <c r="W95" s="1">
+        <v>3.9412917374193097E-15</v>
+      </c>
+      <c r="X95" s="1">
+        <v>7.32747196252603E-15</v>
+      </c>
+      <c r="Y95" s="1">
+        <v>1.77802217393719E-13</v>
+      </c>
+      <c r="Z95" s="1">
+        <v>4.3853809472693699E-15</v>
+      </c>
+      <c r="AA95" s="1">
+        <v>4.4582393332603903E-16</v>
+      </c>
+      <c r="AB95" s="1">
+        <v>2.2370993946196901E-14</v>
+      </c>
+      <c r="AC95" s="1">
+        <v>1.3211653993039401E-14</v>
+      </c>
+      <c r="AD95" s="1">
+        <v>7.5677195558701495E-57</v>
+      </c>
+      <c r="AE95" s="1">
+        <v>8.3821838359199303E-15</v>
+      </c>
+      <c r="AF95" s="1">
+        <v>8.3877349510430602E-14</v>
+      </c>
+      <c r="AG95" s="1">
+        <v>6.10622663543836E-16</v>
+      </c>
+      <c r="AH95" s="1">
+        <v>2.8865798640254102E-15</v>
+      </c>
+      <c r="AI95" s="1">
+        <v>3.3861802251067298E-15</v>
+      </c>
+      <c r="AJ95" s="1">
+        <v>1.6653345369377301E-15</v>
+      </c>
+      <c r="AK95" s="1">
+        <v>4.49640324973188E-15</v>
+      </c>
+      <c r="AL95" s="1">
+        <v>3.6637359812630197E-15</v>
+      </c>
+      <c r="AM95" s="1">
+        <v>1.9767174008755701E-14</v>
+      </c>
+      <c r="AN95" s="1">
+        <v>6.1617377866696204E-15</v>
+      </c>
+      <c r="AO95" s="1">
+        <v>2.6090241078691198E-15</v>
+      </c>
+      <c r="AP95" s="1">
+        <v>2.2204460492503101E-16</v>
+      </c>
+      <c r="AQ95" s="1">
+        <v>1.6653345369377301E-15</v>
+      </c>
+      <c r="AR95" s="1">
+        <v>2.2204460492503101E-16</v>
+      </c>
+      <c r="AS95" s="1">
+        <v>1.4157078287446701E-14</v>
+      </c>
+      <c r="AT95" s="1">
+        <v>5.2735593669694896E-15</v>
+      </c>
+      <c r="AU95" s="1">
+        <v>3.6082248300317603E-15</v>
+      </c>
+      <c r="AV95" s="1">
+        <v>8.3266726846886701E-16</v>
+      </c>
+      <c r="AW95" s="1">
+        <v>1.8873791418627701E-15</v>
+      </c>
+      <c r="AX95" s="1">
+        <v>1.27675647831893E-15</v>
+      </c>
+      <c r="AY95" s="1">
+        <v>9.4368957093138306E-15</v>
+      </c>
+      <c r="AZ95" s="1">
+        <v>1.8873791418627701E-15</v>
+      </c>
+      <c r="BA95" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1664315346937574E-14</v>
+      </c>
+      <c r="BB95" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7298158841423491E-14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A96" s="2"/>
+      <c r="B96" t="s">
+        <v>52</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2.9283202285055101E-73</v>
+      </c>
+      <c r="D96" s="1">
+        <v>1.6212033798227799E-74</v>
+      </c>
+      <c r="E96" s="1">
+        <v>1.9684873134310398E-71</v>
+      </c>
+      <c r="F96" s="1">
+        <v>2.1444212506445201E-71</v>
+      </c>
+      <c r="G96" s="1">
+        <v>1.99364028307843E-69</v>
+      </c>
+      <c r="H96" s="1">
+        <v>3.1499630414622101E-69</v>
+      </c>
+      <c r="I96" s="1">
+        <v>4.42370186743082E-69</v>
+      </c>
+      <c r="J96" s="1">
+        <v>5.8276332679977103E-71</v>
+      </c>
+      <c r="K96" s="1">
+        <v>3.5537488119451202E-75</v>
+      </c>
+      <c r="L96" s="1">
+        <v>1.18169087797676E-69</v>
+      </c>
+      <c r="M96" s="1">
+        <v>9.4505205255780607E-72</v>
+      </c>
+      <c r="N96" s="1">
+        <v>8.6152420622121302E-75</v>
+      </c>
+      <c r="O96" s="1">
+        <v>1.8484398319368099E-71</v>
+      </c>
+      <c r="P96" s="1">
+        <v>4.6448570747438103E-72</v>
+      </c>
+      <c r="Q96" s="1">
+        <v>5.6895722163288296E-73</v>
+      </c>
+      <c r="R96" s="1">
+        <v>5.3845734482812998E-73</v>
+      </c>
+      <c r="S96" s="1">
+        <v>1.5032897786428799E-70</v>
+      </c>
+      <c r="T96" s="1">
+        <v>9.6866887458607491E-72</v>
+      </c>
+      <c r="U96" s="1">
+        <v>6.9864393506227698E-72</v>
+      </c>
+      <c r="V96" s="1">
+        <v>2.4026902615229599E-67</v>
+      </c>
+      <c r="W96" s="1">
+        <v>1.88339942217002E-74</v>
+      </c>
+      <c r="X96" s="1">
+        <v>1.19392673378172E-70</v>
+      </c>
+      <c r="Y96" s="1">
+        <v>3.7977405924820701E-73</v>
+      </c>
+      <c r="Z96" s="1">
+        <v>6.7146944395032596E-70</v>
+      </c>
+      <c r="AA96" s="1">
+        <v>3.6197426666776898E-75</v>
+      </c>
+      <c r="AB96" s="1">
+        <v>6.8105934042044695E-72</v>
+      </c>
+      <c r="AC96" s="1">
+        <v>5.4720466899502096E-75</v>
+      </c>
+      <c r="AD96" s="1">
+        <v>2.5119240324931001E-71</v>
+      </c>
+      <c r="AE96" s="1">
+        <v>1.15535048812275E-71</v>
+      </c>
+      <c r="AF96" s="1">
+        <v>4.9732925417050096E-71</v>
+      </c>
+      <c r="AG96" s="1">
+        <v>2.7091386332912898E-71</v>
+      </c>
+      <c r="AH96" s="1">
+        <v>1.11140500712471E-73</v>
+      </c>
+      <c r="AI96" s="1">
+        <v>9.4361952395204197E-72</v>
+      </c>
+      <c r="AJ96" s="1">
+        <v>2.2646807392695299E-71</v>
+      </c>
+      <c r="AK96" s="1">
+        <v>3.9033629914715298E-71</v>
+      </c>
+      <c r="AL96" s="1">
+        <v>1.0859012774985701E-71</v>
+      </c>
+      <c r="AM96" s="1">
+        <v>2.4916824900531499E-72</v>
+      </c>
+      <c r="AN96" s="1">
+        <v>9.1123490446650906E-74</v>
+      </c>
+      <c r="AO96" s="1">
+        <v>5.7883506097866797E-71</v>
+      </c>
+      <c r="AP96" s="1">
+        <v>6.8284341763814496E-71</v>
+      </c>
+      <c r="AQ96" s="1">
+        <v>2.21555283281949E-76</v>
+      </c>
+      <c r="AR96" s="1">
+        <v>1.4611532249653099E-71</v>
+      </c>
+      <c r="AS96" s="1">
+        <v>4.2936072615186401E-73</v>
+      </c>
+      <c r="AT96" s="1">
+        <v>2.0963280124947E-73</v>
+      </c>
+      <c r="AU96" s="1">
+        <v>6.5792786969925304E-71</v>
+      </c>
+      <c r="AV96" s="1">
+        <v>2.5931785715216999E-71</v>
+      </c>
+      <c r="AW96" s="1">
+        <v>1.9743859914394798E-71</v>
+      </c>
+      <c r="AX96" s="1">
+        <v>9.8597873298931908E-69</v>
+      </c>
+      <c r="AY96" s="1">
+        <v>1.82932950669545E-70</v>
+      </c>
+      <c r="AZ96" s="1">
+        <v>1.8460235956082402E-71</v>
+      </c>
+      <c r="BA96" s="1">
+        <f t="shared" si="2"/>
+        <v>5.2525750550741331E-69</v>
+      </c>
+      <c r="BB96" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3610222181465058E-68</v>
+      </c>
+    </row>
+    <row r="97" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A97" s="2"/>
+      <c r="B97" t="s">
+        <v>53</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0.160738698826772</v>
+      </c>
+      <c r="D97" s="1">
+        <v>4.1902087514238602</v>
+      </c>
+      <c r="E97" s="1">
+        <v>3.33945588769418</v>
+      </c>
+      <c r="F97" s="1">
+        <v>4.1719904005010501E-2</v>
+      </c>
+      <c r="G97" s="1">
+        <v>3.9622594315686999</v>
+      </c>
+      <c r="H97" s="1">
+        <v>3.5319255230672</v>
+      </c>
+      <c r="I97" s="1">
+        <v>4.2907879899427801</v>
+      </c>
+      <c r="J97" s="1">
+        <v>10.1956154572811</v>
+      </c>
+      <c r="K97" s="1">
+        <v>3.4923371263940202</v>
+      </c>
+      <c r="L97" s="1">
+        <v>90004.367187777796</v>
+      </c>
+      <c r="M97" s="1">
+        <v>5.0870433673547399</v>
+      </c>
+      <c r="N97" s="1">
+        <v>4.4982255061067704</v>
+      </c>
+      <c r="O97" s="1">
+        <v>3022.4769953912</v>
+      </c>
+      <c r="P97" s="1">
+        <v>3.13630907584347</v>
+      </c>
+      <c r="Q97" s="1">
+        <v>26.204863582198101</v>
+      </c>
+      <c r="R97" s="1">
+        <v>4.5550031287587096</v>
+      </c>
+      <c r="S97" s="1">
+        <v>2.5938289613448799</v>
+      </c>
+      <c r="T97" s="1">
+        <v>4.5884613889410897</v>
+      </c>
+      <c r="U97" s="1">
+        <v>1.7359413319424</v>
+      </c>
+      <c r="V97" s="1">
+        <v>6.1131324505935298</v>
+      </c>
+      <c r="W97" s="1">
+        <v>3.58474943848028</v>
+      </c>
+      <c r="X97" s="1">
+        <v>1.0836966102812</v>
+      </c>
+      <c r="Y97" s="1">
+        <v>3.58316365824968</v>
+      </c>
+      <c r="Z97" s="1">
+        <v>4.6993746454577501</v>
+      </c>
+      <c r="AA97" s="1">
+        <v>7.7611827600616596</v>
+      </c>
+      <c r="AB97" s="1">
+        <v>3.7059823765543398</v>
+      </c>
+      <c r="AC97" s="1">
+        <v>5.5720606862125504</v>
+      </c>
+      <c r="AD97" s="1">
+        <v>3.8178198064778699</v>
+      </c>
+      <c r="AE97" s="1">
+        <v>1.35540130029648</v>
+      </c>
+      <c r="AF97" s="1">
+        <v>0.21736480827931001</v>
+      </c>
+      <c r="AG97" s="1">
+        <v>3.6038825564041899</v>
+      </c>
+      <c r="AH97" s="1">
+        <v>4.28163074626391</v>
+      </c>
+      <c r="AI97" s="1">
+        <v>6.4898409559958399</v>
+      </c>
+      <c r="AJ97" s="1">
+        <v>22.191704609663301</v>
+      </c>
+      <c r="AK97" s="1">
+        <v>60.019814748787098</v>
+      </c>
+      <c r="AL97" s="1">
+        <v>6.0880583654223303E-2</v>
+      </c>
+      <c r="AM97" s="1">
+        <v>1.0366229452814699</v>
+      </c>
+      <c r="AN97" s="1">
+        <v>1.1185405683309799</v>
+      </c>
+      <c r="AO97" s="1">
+        <v>4.3681051918013303</v>
+      </c>
+      <c r="AP97" s="1">
+        <v>4.3128069717270803</v>
+      </c>
+      <c r="AQ97" s="1">
+        <v>2.6293428887950601</v>
+      </c>
+      <c r="AR97" s="1">
+        <v>1.7689794902590199</v>
+      </c>
+      <c r="AS97" s="1">
+        <v>3019.1276345803199</v>
+      </c>
+      <c r="AT97" s="1">
+        <v>131.41992202869801</v>
+      </c>
+      <c r="AU97" s="1">
+        <v>1.59141175986546</v>
+      </c>
+      <c r="AV97" s="1">
+        <v>4.0808808738820499</v>
+      </c>
+      <c r="AW97" s="1">
+        <v>5.4502448046195697</v>
+      </c>
+      <c r="AX97" s="1">
+        <v>4.5874081744834001</v>
+      </c>
+      <c r="AY97" s="1">
+        <v>3.5259863744374602</v>
+      </c>
+      <c r="AZ97" s="1">
+        <v>90002.243942086599</v>
+      </c>
+      <c r="BA97" s="1">
+        <f t="shared" si="2"/>
+        <v>3728.7570483952495</v>
+      </c>
+      <c r="BB97" s="1">
+        <f t="shared" si="3"/>
+        <v>17620.602620458147</v>
+      </c>
+    </row>
+    <row r="98" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A98" s="2"/>
+      <c r="B98" t="s">
+        <v>54</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1.10983467393134E-44</v>
+      </c>
+      <c r="D98" s="1">
+        <v>5.5972686517397398E-44</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1.48937994542409E-47</v>
+      </c>
+      <c r="F98" s="1">
+        <v>1.28282607884506E-44</v>
+      </c>
+      <c r="G98" s="1">
+        <v>8.6234407221859605E-45</v>
+      </c>
+      <c r="H98" s="1">
+        <v>4.7991369423038403E-46</v>
+      </c>
+      <c r="I98" s="1">
+        <v>9.2883786490949506E-45</v>
+      </c>
+      <c r="J98" s="1">
+        <v>1.11439704913752E-44</v>
+      </c>
+      <c r="K98" s="1">
+        <v>1.8210132084823298E-43</v>
+      </c>
+      <c r="L98" s="1">
+        <v>1.30001925611235E-43</v>
+      </c>
+      <c r="M98" s="1">
+        <v>6.2132111069279997E-45</v>
+      </c>
+      <c r="N98" s="1">
+        <v>1.1738750967105E-44</v>
+      </c>
+      <c r="O98" s="1">
+        <v>2.2399496102448401E-44</v>
+      </c>
+      <c r="P98" s="1">
+        <v>2.1057293173598201E-44</v>
+      </c>
+      <c r="Q98" s="1">
+        <v>2.1693178083843099E-44</v>
+      </c>
+      <c r="R98" s="1">
+        <v>1.46612415165203E-43</v>
+      </c>
+      <c r="S98" s="1">
+        <v>4.3109019118700698E-45</v>
+      </c>
+      <c r="T98" s="1">
+        <v>1.0418216095528501E-43</v>
+      </c>
+      <c r="U98" s="1">
+        <v>7.4731822866504102E-47</v>
+      </c>
+      <c r="V98" s="1">
+        <v>4.7160192400190103E-43</v>
+      </c>
+      <c r="W98" s="1">
+        <v>2.4114533484567898E-43</v>
+      </c>
+      <c r="X98" s="1">
+        <v>1.12033553442304E-44</v>
+      </c>
+      <c r="Y98" s="1">
+        <v>8.3091695757079405E-45</v>
+      </c>
+      <c r="Z98" s="1">
+        <v>1.1845154438911799E-43</v>
+      </c>
+      <c r="AA98" s="1">
+        <v>3.6591097186971898E-46</v>
+      </c>
+      <c r="AB98" s="1">
+        <v>6.1738257380537103E-44</v>
+      </c>
+      <c r="AC98" s="1">
+        <v>5.93011030510027E-45</v>
+      </c>
+      <c r="AD98" s="1">
+        <v>9.1612652684580597E-44</v>
+      </c>
+      <c r="AE98" s="1">
+        <v>4.2818587744463197E-45</v>
+      </c>
+      <c r="AF98" s="1">
+        <v>5.2509788437581403E-44</v>
+      </c>
+      <c r="AG98" s="1">
+        <v>2.7601390757316099E-43</v>
+      </c>
+      <c r="AH98" s="1">
+        <v>4.6526513666022199E-44</v>
+      </c>
+      <c r="AI98" s="1">
+        <v>1.9517710631605E-44</v>
+      </c>
+      <c r="AJ98" s="1">
+        <v>5.01822719388669E-44</v>
+      </c>
+      <c r="AK98" s="1">
+        <v>2.6311677823534501E-42</v>
+      </c>
+      <c r="AL98" s="1">
+        <v>1.12575464839312E-45</v>
+      </c>
+      <c r="AM98" s="1">
+        <v>2.2696639482218E-45</v>
+      </c>
+      <c r="AN98" s="1">
+        <v>3.1286902434018598E-44</v>
+      </c>
+      <c r="AO98" s="1">
+        <v>9.0182281024111796E-45</v>
+      </c>
+      <c r="AP98" s="1">
+        <v>4.15950718030755E-44</v>
+      </c>
+      <c r="AQ98" s="1">
+        <v>4.3515477782200501E-44</v>
+      </c>
+      <c r="AR98" s="1">
+        <v>4.4630064076256096E-43</v>
+      </c>
+      <c r="AS98" s="1">
+        <v>2.1491233112745301E-43</v>
+      </c>
+      <c r="AT98" s="1">
+        <v>1.0319621915253699E-45</v>
+      </c>
+      <c r="AU98" s="1">
+        <v>1.8875453261959E-43</v>
+      </c>
+      <c r="AV98" s="1">
+        <v>1.27990375540651E-43</v>
+      </c>
+      <c r="AW98" s="1">
+        <v>1.38244877659742E-43</v>
+      </c>
+      <c r="AX98" s="1">
+        <v>1.3697655917516601E-44</v>
+      </c>
+      <c r="AY98" s="1">
+        <v>1.9055922258491901E-44</v>
+      </c>
+      <c r="AZ98" s="1">
+        <v>2.0372846064213899E-45</v>
+      </c>
+      <c r="BA98" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2262460102852502E-43</v>
+      </c>
+      <c r="BB98" s="1">
+        <f t="shared" si="3"/>
+        <v>3.7340911546524885E-43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A99" s="2"/>
+      <c r="B99" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1.7125425911264801E-136</v>
+      </c>
+      <c r="D99" s="1">
+        <v>2.6018857941927702E-128</v>
+      </c>
+      <c r="E99" s="1">
+        <v>7.1002111015423803E-129</v>
+      </c>
+      <c r="F99" s="1">
+        <v>2.05388201927333E-128</v>
+      </c>
+      <c r="G99" s="1">
+        <v>3.5767302751284702E-127</v>
+      </c>
+      <c r="H99" s="1">
+        <v>2.4871132532854101E-131</v>
+      </c>
+      <c r="I99" s="1">
+        <v>1.4770228415214201E-128</v>
+      </c>
+      <c r="J99" s="1">
+        <v>2.5978867050539798E-128</v>
+      </c>
+      <c r="K99" s="1">
+        <v>1.66659421728225E-131</v>
+      </c>
+      <c r="L99" s="1">
+        <v>2.3470271646368399E-125</v>
+      </c>
+      <c r="M99" s="1">
+        <v>2.41488366935878E-136</v>
+      </c>
+      <c r="N99" s="1">
+        <v>1.2384894535148301E-133</v>
+      </c>
+      <c r="O99" s="1">
+        <v>1.1508050318193701E-127</v>
+      </c>
+      <c r="P99" s="1">
+        <v>1.1941405694694299E-121</v>
+      </c>
+      <c r="Q99" s="1">
+        <v>2.0012268209761101E-122</v>
+      </c>
+      <c r="R99" s="1">
+        <v>1.11973498573756E-125</v>
+      </c>
+      <c r="S99" s="1">
+        <v>3.66493681469419E-123</v>
+      </c>
+      <c r="T99" s="1">
+        <v>1.52263241724461E-130</v>
+      </c>
+      <c r="U99" s="1">
+        <v>2.04415074860436E-128</v>
+      </c>
+      <c r="V99" s="1">
+        <v>1.3128818165543599E-134</v>
+      </c>
+      <c r="W99" s="1">
+        <v>1.7960851297321399E-122</v>
+      </c>
+      <c r="X99" s="1">
+        <v>3.0616924716932302E-132</v>
+      </c>
+      <c r="Y99" s="1">
+        <v>7.6003371386683399E-134</v>
+      </c>
+      <c r="Z99" s="1">
+        <v>3.4725455475345799E-124</v>
+      </c>
+      <c r="AA99" s="1">
+        <v>1.4057864835328901E-126</v>
+      </c>
+      <c r="AB99" s="1">
+        <v>9.9164604135439504E-121</v>
+      </c>
+      <c r="AC99" s="1">
+        <v>2.1537441210138599E-118</v>
+      </c>
+      <c r="AD99" s="1">
+        <v>3.1146793342090301E-127</v>
+      </c>
+      <c r="AE99" s="1">
+        <v>1.65466306701399E-134</v>
+      </c>
+      <c r="AF99" s="1">
+        <v>6.5936416798532996E-125</v>
+      </c>
+      <c r="AG99" s="1">
+        <v>3.9008564678620499E-124</v>
+      </c>
+      <c r="AH99" s="1">
+        <v>5.1910512033695997E-127</v>
+      </c>
+      <c r="AI99" s="1">
+        <v>3.45758705103165E-128</v>
+      </c>
+      <c r="AJ99" s="1">
+        <v>8.1159278543775496E-131</v>
+      </c>
+      <c r="AK99" s="1">
+        <v>3.79892821820465E-125</v>
+      </c>
+      <c r="AL99" s="1">
+        <v>2.0949193362268101E-134</v>
+      </c>
+      <c r="AM99" s="1">
+        <v>4.0882203745343999E-134</v>
+      </c>
+      <c r="AN99" s="1">
+        <v>3.0354263796449401E-131</v>
+      </c>
+      <c r="AO99" s="1">
+        <v>6.1860290097875397E-131</v>
+      </c>
+      <c r="AP99" s="1">
+        <v>2.4993690905362902E-128</v>
+      </c>
+      <c r="AQ99" s="1">
+        <v>6.5656378588321899E-129</v>
+      </c>
+      <c r="AR99" s="1">
+        <v>2.6926217408986199E-121</v>
+      </c>
+      <c r="AS99" s="1">
+        <v>1.23251494105161E-126</v>
+      </c>
+      <c r="AT99" s="1">
+        <v>9.2739732981404801E-130</v>
+      </c>
+      <c r="AU99" s="1">
+        <v>1.5125691988540901E-130</v>
+      </c>
+      <c r="AV99" s="1">
+        <v>1.81354208692268E-127</v>
+      </c>
+      <c r="AW99" s="1">
+        <v>6.1077126922949204E-123</v>
+      </c>
+      <c r="AX99" s="1">
+        <v>5.7776239389371599E-125</v>
+      </c>
+      <c r="AY99" s="1">
+        <v>1.2732821688386599E-126</v>
+      </c>
+      <c r="AZ99" s="1">
+        <v>2.6463347800959898E-125</v>
+      </c>
+      <c r="BA99" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3360689178919534E-120</v>
+      </c>
+      <c r="BB99" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0148676124430789E-119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
+      <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+      <c r="Y100" s="1"/>
+      <c r="Z100" s="1"/>
+      <c r="AA100" s="1"/>
+      <c r="AB100" s="1"/>
+      <c r="AC100" s="1"/>
+      <c r="AD100" s="1"/>
+      <c r="AE100" s="1"/>
+      <c r="AF100" s="1"/>
+      <c r="AG100" s="1"/>
+      <c r="AH100" s="1"/>
+      <c r="AI100" s="1"/>
+      <c r="AJ100" s="1"/>
+      <c r="AK100" s="1"/>
+      <c r="AL100" s="1"/>
+      <c r="AM100" s="1"/>
+      <c r="AN100" s="1"/>
+      <c r="AO100" s="1"/>
+      <c r="AP100" s="1"/>
+      <c r="AQ100" s="1"/>
+      <c r="AR100" s="1"/>
+      <c r="AS100" s="1"/>
+      <c r="AT100" s="1"/>
+      <c r="AU100" s="1"/>
+      <c r="AV100" s="1"/>
+      <c r="AW100" s="1"/>
+      <c r="AX100" s="1"/>
+      <c r="AY100" s="1"/>
+      <c r="AZ100" s="1"/>
+      <c r="BA100" s="1"/>
+      <c r="BB100" s="1"/>
+    </row>
+    <row r="101" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B101" t="s">
+        <v>48</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2.3858603981352598E-10</v>
+      </c>
+      <c r="D101" s="1">
+        <v>2.9444890969898597E-11</v>
+      </c>
+      <c r="E101" s="1">
+        <v>4.1428194208492603E-11</v>
+      </c>
+      <c r="F101" s="1">
+        <v>3.0668445560877398E-10</v>
+      </c>
+      <c r="G101" s="1">
+        <v>19.9547693877015</v>
+      </c>
+      <c r="H101" s="1">
+        <v>2.21902496377879E-11</v>
+      </c>
+      <c r="I101" s="1">
+        <v>3.69350772189137E-10</v>
+      </c>
+      <c r="J101" s="1">
+        <v>2.9096725029376099E-11</v>
+      </c>
+      <c r="K101" s="1">
+        <v>19.6457700861862</v>
+      </c>
+      <c r="L101" s="1">
+        <v>8.4696694102603903E-11</v>
+      </c>
+      <c r="M101" s="1">
+        <v>1.11821663040246E-10</v>
+      </c>
+      <c r="N101" s="1">
+        <v>7.47455430882837E-11</v>
+      </c>
+      <c r="O101" s="1">
+        <v>1.3625012229567801E-10</v>
+      </c>
+      <c r="P101" s="1">
+        <v>9.3272944923228403E-11</v>
+      </c>
+      <c r="Q101" s="1">
+        <v>3.1295854796553602E-10</v>
+      </c>
+      <c r="R101" s="1">
+        <v>2.07350581149512E-10</v>
+      </c>
+      <c r="S101" s="1">
+        <v>1.64675384439761E-10</v>
+      </c>
+      <c r="T101" s="1">
+        <v>3.1473490480493599E-11</v>
+      </c>
+      <c r="U101" s="1">
+        <v>5.0939874540745202E-10</v>
+      </c>
+      <c r="V101" s="1">
+        <v>2.88480350718601E-11</v>
+      </c>
+      <c r="W101" s="1">
+        <v>2.0588331040016801E-10</v>
+      </c>
+      <c r="X101" s="1">
+        <v>9.4150820473259997E-10</v>
+      </c>
+      <c r="Y101" s="1">
+        <v>5.49547962691577E-10</v>
+      </c>
+      <c r="Z101" s="1">
+        <v>3.1832314562052501E-11</v>
+      </c>
+      <c r="AA101" s="1">
+        <v>3.6908431866322598E-10</v>
+      </c>
+      <c r="AB101" s="1">
+        <v>1.92802218634824E-10</v>
+      </c>
+      <c r="AC101" s="1">
+        <v>5.4198778798308901E-10</v>
+      </c>
+      <c r="AD101" s="1">
+        <v>1.7462298274040199E-10</v>
+      </c>
+      <c r="AE101" s="1">
+        <v>7.7765349715264204E-11</v>
+      </c>
+      <c r="AF101" s="1">
+        <v>6.8016703380635603E-11</v>
+      </c>
+      <c r="AG101" s="1">
+        <v>5.8307136896473795E-11</v>
+      </c>
+      <c r="AH101" s="1">
+        <v>4.1378811488357299E-10</v>
+      </c>
+      <c r="AI101" s="1">
+        <v>1.81199055759862E-10</v>
+      </c>
+      <c r="AJ101" s="1">
+        <v>1.6662582424942201E-10</v>
+      </c>
+      <c r="AK101" s="1">
+        <v>2.09862349720424E-10</v>
+      </c>
+      <c r="AL101" s="1">
+        <v>8.6497919937755796E-11</v>
+      </c>
+      <c r="AM101" s="1">
+        <v>1.76825665221259E-10</v>
+      </c>
+      <c r="AN101" s="1">
+        <v>1.6304824157487001E-10</v>
+      </c>
+      <c r="AO101" s="1">
+        <v>8.5801588056710898E-11</v>
+      </c>
+      <c r="AP101" s="1">
+        <v>8.6917140151854294E-11</v>
+      </c>
+      <c r="AQ101" s="1">
+        <v>7.7303177192789008E-9</v>
+      </c>
+      <c r="AR101" s="1">
+        <v>1.38200562105339E-11</v>
+      </c>
+      <c r="AS101" s="1">
+        <v>4.30105728810304E-10</v>
+      </c>
+      <c r="AT101" s="1">
+        <v>6.4343197436755898E-11</v>
+      </c>
+      <c r="AU101" s="1">
+        <v>2.56076049254261E-10</v>
+      </c>
+      <c r="AV101" s="1">
+        <v>9.2502361326296502E-10</v>
+      </c>
+      <c r="AW101" s="1">
+        <v>6.2851057691659701E-11</v>
+      </c>
+      <c r="AX101" s="1">
+        <v>1.3838530321663701E-10</v>
+      </c>
+      <c r="AY101" s="1">
+        <v>4.7283066351155899E-11</v>
+      </c>
+      <c r="AZ101" s="1">
+        <v>4.3428727281025198E-10</v>
+      </c>
+      <c r="BA101" s="1">
+        <f t="shared" si="2"/>
+        <v>0.79201078983128814</v>
+      </c>
+      <c r="BB101" s="1">
+        <f t="shared" si="3"/>
+        <v>3.8801676485306107</v>
+      </c>
+    </row>
+    <row r="102" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A102" s="2"/>
+      <c r="B102" t="s">
+        <v>49</v>
+      </c>
+      <c r="C102" s="1">
+        <v>40.793265879376897</v>
+      </c>
+      <c r="D102" s="1">
+        <v>45.768061164843402</v>
+      </c>
+      <c r="E102" s="1">
+        <v>86.394981325583004</v>
+      </c>
+      <c r="F102" s="1">
+        <v>27.8588384851552</v>
+      </c>
+      <c r="G102" s="1">
+        <v>42.783163796852897</v>
+      </c>
+      <c r="H102" s="1">
+        <v>27.858833447335801</v>
+      </c>
+      <c r="I102" s="1">
+        <v>90.540716786280498</v>
+      </c>
+      <c r="J102" s="1">
+        <v>56.712553429344403</v>
+      </c>
+      <c r="K102" s="1">
+        <v>47.760968019563897</v>
+      </c>
+      <c r="L102" s="1">
+        <v>62.6821166804584</v>
+      </c>
+      <c r="M102" s="1">
+        <v>64.672227788167902</v>
+      </c>
+      <c r="N102" s="1">
+        <v>74.621666540675506</v>
+      </c>
+      <c r="O102" s="1">
+        <v>56.712590641593302</v>
+      </c>
+      <c r="P102" s="1">
+        <v>34.823521612455302</v>
+      </c>
+      <c r="Q102" s="1">
+        <v>44.773081911035597</v>
+      </c>
+      <c r="R102" s="1">
+        <v>57.707509305257702</v>
+      </c>
+      <c r="S102" s="1">
+        <v>22.884043278113001</v>
+      </c>
+      <c r="T102" s="1">
+        <v>56.7125298685865</v>
+      </c>
+      <c r="U102" s="1">
+        <v>39.798327018998101</v>
+      </c>
+      <c r="V102" s="1">
+        <v>53.7276781147036</v>
+      </c>
+      <c r="W102" s="1">
+        <v>77.606487423400594</v>
+      </c>
+      <c r="X102" s="1">
+        <v>19.899196278029098</v>
+      </c>
+      <c r="Y102" s="1">
+        <v>43.778122853942399</v>
+      </c>
+      <c r="Z102" s="1">
+        <v>36.8182623991813</v>
+      </c>
+      <c r="AA102" s="1">
+        <v>77.440364925200498</v>
+      </c>
+      <c r="AB102" s="1">
+        <v>27.858838485154902</v>
+      </c>
+      <c r="AC102" s="1">
+        <v>50.742826177957298</v>
+      </c>
+      <c r="AD102" s="1">
+        <v>62.682233742045597</v>
+      </c>
+      <c r="AE102" s="1">
+        <v>40.793200143195499</v>
+      </c>
+      <c r="AF102" s="1">
+        <v>26.863879428061601</v>
+      </c>
+      <c r="AG102" s="1">
+        <v>90.374751743096695</v>
+      </c>
+      <c r="AH102" s="1">
+        <v>33.828587842624003</v>
+      </c>
+      <c r="AI102" s="1">
+        <v>42.783123220523201</v>
+      </c>
+      <c r="AJ102" s="1">
+        <v>43.778072201978297</v>
+      </c>
+      <c r="AK102" s="1">
+        <v>77.6064571510489</v>
+      </c>
+      <c r="AL102" s="1">
+        <v>32.833628732802303</v>
+      </c>
+      <c r="AM102" s="1">
+        <v>51.737800393945903</v>
+      </c>
+      <c r="AN102" s="1">
+        <v>51.737785235050502</v>
+      </c>
+      <c r="AO102" s="1">
+        <v>22.884043241788699</v>
+      </c>
+      <c r="AP102" s="1">
+        <v>25.868920370968301</v>
+      </c>
+      <c r="AQ102" s="1">
+        <v>41.788245432649099</v>
+      </c>
+      <c r="AR102" s="1">
+        <v>34.8235216125926</v>
+      </c>
+      <c r="AS102" s="1">
+        <v>35.818480669548599</v>
+      </c>
+      <c r="AT102" s="1">
+        <v>85.400062661918597</v>
+      </c>
+      <c r="AU102" s="1">
+        <v>33.828572631000299</v>
+      </c>
+      <c r="AV102" s="1">
+        <v>55.717616425604596</v>
+      </c>
+      <c r="AW102" s="1">
+        <v>48.586622889838502</v>
+      </c>
+      <c r="AX102" s="1">
+        <v>43.778143050656801</v>
+      </c>
+      <c r="AY102" s="1">
+        <v>60.692137793232199</v>
+      </c>
+      <c r="AZ102" s="1">
+        <v>32.833603498268999</v>
+      </c>
+      <c r="BA102" s="1">
+        <f t="shared" si="2"/>
+        <v>48.935405274993748</v>
+      </c>
+      <c r="BB102" s="1">
+        <f t="shared" si="3"/>
+        <v>18.495199439816783</v>
+      </c>
+    </row>
+    <row r="103" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A103" s="2"/>
+      <c r="B103" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0</v>
+      </c>
+      <c r="E103" s="1">
+        <v>7.3960403341150104E-3</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0</v>
+      </c>
+      <c r="G103" s="1">
+        <v>9.8572846078208692E-3</v>
+      </c>
+      <c r="H103" s="1">
+        <v>1.9689998004848198E-2</v>
+      </c>
+      <c r="I103" s="1">
+        <v>1.7236111917661601E-2</v>
+      </c>
+      <c r="J103" s="1">
+        <v>1.7226293859712902E-2</v>
+      </c>
+      <c r="K103" s="1">
+        <v>0</v>
+      </c>
+      <c r="L103" s="1">
+        <v>3.6901669577180697E-2</v>
+      </c>
+      <c r="M103" s="1">
+        <v>2.95653634100005E-2</v>
+      </c>
+      <c r="N103" s="1">
+        <v>0</v>
+      </c>
+      <c r="O103" s="1">
+        <v>0</v>
+      </c>
+      <c r="P103" s="1">
+        <v>4.1718958797780203E-2</v>
+      </c>
+      <c r="Q103" s="1">
+        <v>1.9719489248184799E-2</v>
+      </c>
+      <c r="R103" s="1">
+        <v>0</v>
+      </c>
+      <c r="S103" s="1">
+        <v>3.4384062210073299E-2</v>
+      </c>
+      <c r="T103" s="1">
+        <v>0</v>
+      </c>
+      <c r="U103" s="1">
+        <v>1.47797767548257E-2</v>
+      </c>
+      <c r="V103" s="1">
+        <v>9.8646720610061599E-3</v>
+      </c>
+      <c r="W103" s="1">
+        <v>0</v>
+      </c>
+      <c r="X103" s="1">
+        <v>1.23160725192616E-2</v>
+      </c>
+      <c r="Y103" s="1">
+        <v>1.23160725192616E-2</v>
+      </c>
+      <c r="Z103" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA103" s="1">
+        <v>7.3960403341149002E-3</v>
+      </c>
+      <c r="AB103" s="1">
+        <v>2.46026825568612E-2</v>
+      </c>
+      <c r="AC103" s="1">
+        <v>1.96777345580375E-2</v>
+      </c>
+      <c r="AD103" s="1">
+        <v>4.4058431386214597E-2</v>
+      </c>
+      <c r="AE103" s="1">
+        <v>1.23160725192617E-2</v>
+      </c>
+      <c r="AF103" s="1">
+        <v>3.9382435243166397E-2</v>
+      </c>
+      <c r="AG103" s="1">
+        <v>3.4462404160991597E-2</v>
+      </c>
+      <c r="AH103" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI103" s="1">
+        <v>2.2156143668715302E-2</v>
+      </c>
+      <c r="AJ103" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK103" s="1">
+        <v>3.9201655465125398E-2</v>
+      </c>
+      <c r="AL103" s="1">
+        <v>7.8333527431545993E-2</v>
+      </c>
+      <c r="AM103" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN103" s="1">
+        <v>2.46026825568612E-2</v>
+      </c>
+      <c r="AO103" s="1">
+        <v>1.4772407756803101E-2</v>
+      </c>
+      <c r="AP103" s="1">
+        <v>9.8572846078207599E-3</v>
+      </c>
+      <c r="AQ103" s="1">
+        <v>3.2006110385265803E-2</v>
+      </c>
+      <c r="AR103" s="1">
+        <v>1.7226293859712902E-2</v>
+      </c>
+      <c r="AS103" s="1">
+        <v>1.23209888751067E-2</v>
+      </c>
+      <c r="AT103" s="1">
+        <v>3.4384062210073299E-2</v>
+      </c>
+      <c r="AU103" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV103" s="1">
+        <v>1.23209888751066E-2</v>
+      </c>
+      <c r="AW103" s="1">
+        <v>7.3960403341149002E-3</v>
+      </c>
+      <c r="AX103" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY103" s="1">
+        <v>3.4401154367839797E-2</v>
+      </c>
+      <c r="AZ103" s="1">
+        <v>2.70663642877512E-2</v>
+      </c>
+      <c r="BA103" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6618267425244474E-2</v>
+      </c>
+      <c r="BB103" s="1">
+        <f t="shared" si="3"/>
+        <v>1.6268076505336401E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A104" s="2"/>
+      <c r="B104" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" s="1">
+        <v>4.4402111088937399</v>
+      </c>
+      <c r="D104" s="1">
+        <v>7.4524558380963695E-14</v>
+      </c>
+      <c r="E104" s="1">
+        <v>4.4402111088937701</v>
+      </c>
+      <c r="F104" s="1">
+        <v>7.0485518448412795E-14</v>
+      </c>
+      <c r="G104" s="1">
+        <v>1.4036499902529701E-10</v>
+      </c>
+      <c r="H104" s="1">
+        <v>1.02777007741947E-13</v>
+      </c>
+      <c r="I104" s="1">
+        <v>7.3216044243496101E-14</v>
+      </c>
+      <c r="J104" s="1">
+        <v>2.0240524213842699E-14</v>
+      </c>
+      <c r="K104" s="1">
+        <v>1.33628685221481E-13</v>
+      </c>
+      <c r="L104" s="1">
+        <v>1.98229234545194E-14</v>
+      </c>
+      <c r="M104" s="1">
+        <v>2.95495873317768E-14</v>
+      </c>
+      <c r="N104" s="1">
+        <v>1.605414199555E-13</v>
+      </c>
+      <c r="O104" s="1">
+        <v>4.88989124353269E-14</v>
+      </c>
+      <c r="P104" s="1">
+        <v>3.6952409019867201E-14</v>
+      </c>
+      <c r="Q104" s="1">
+        <v>4.4402111088937302</v>
+      </c>
+      <c r="R104" s="1">
+        <v>8.5512882762099706E-14</v>
+      </c>
+      <c r="S104" s="1">
+        <v>3.39758631015028E-14</v>
+      </c>
+      <c r="T104" s="1">
+        <v>6.1353770667157895E-14</v>
+      </c>
+      <c r="U104" s="1">
+        <v>4.4402111088937302</v>
+      </c>
+      <c r="V104" s="1">
+        <v>4.4402111088937497</v>
+      </c>
+      <c r="W104" s="1">
+        <v>4.1713598737040199E-14</v>
+      </c>
+      <c r="X104" s="1">
+        <v>4.4402111088937604</v>
+      </c>
+      <c r="Y104" s="1">
+        <v>4.4402111088937399</v>
+      </c>
+      <c r="Z104" s="1">
+        <v>6.4159889541291503E-14</v>
+      </c>
+      <c r="AA104" s="1">
+        <v>4.4402111088948697</v>
+      </c>
+      <c r="AB104" s="1">
+        <v>4.4402111088937399</v>
+      </c>
+      <c r="AC104" s="1">
+        <v>4.96439381027074E-14</v>
+      </c>
+      <c r="AD104" s="1">
+        <v>7.5106391828987894E-14</v>
+      </c>
+      <c r="AE104" s="1">
+        <v>6.0676679783389503E-14</v>
+      </c>
+      <c r="AF104" s="1">
+        <v>6.2213155211459101E-14</v>
+      </c>
+      <c r="AG104" s="1">
+        <v>9.1810782115285004E-14</v>
+      </c>
+      <c r="AH104" s="1">
+        <v>2.4878084404795002E-13</v>
+      </c>
+      <c r="AI104" s="1">
+        <v>5.0370114858415701E-14</v>
+      </c>
+      <c r="AJ104" s="1">
+        <v>2.4556539190504998E-13</v>
+      </c>
+      <c r="AK104" s="1">
+        <v>2.3798951905318699E-14</v>
+      </c>
+      <c r="AL104" s="1">
+        <v>1.05808253559934E-13</v>
+      </c>
+      <c r="AM104" s="1">
+        <v>3.1667472779321898E-14</v>
+      </c>
+      <c r="AN104" s="1">
+        <v>4.2288647000929902E-14</v>
+      </c>
+      <c r="AO104" s="1">
+        <v>1.26434285287801E-13</v>
+      </c>
+      <c r="AP104" s="1">
+        <v>2.5912499367513199E-13</v>
+      </c>
+      <c r="AQ104" s="1">
+        <v>1.00808465876557E-13</v>
+      </c>
+      <c r="AR104" s="1">
+        <v>3.01367107653019E-14</v>
+      </c>
+      <c r="AS104" s="1">
+        <v>1.4699525643753399E-13</v>
+      </c>
+      <c r="AT104" s="1">
+        <v>3.6104096589603999E-14</v>
+      </c>
+      <c r="AU104" s="1">
+        <v>7.3262806887791404E-14</v>
+      </c>
+      <c r="AV104" s="1">
+        <v>5.85542984672995E-14</v>
+      </c>
+      <c r="AW104" s="1">
+        <v>6.8996343471864198E-14</v>
+      </c>
+      <c r="AX104" s="1">
+        <v>1.2881404193913899E-13</v>
+      </c>
+      <c r="AY104" s="1">
+        <v>6.2079295894098705E-14</v>
+      </c>
+      <c r="AZ104" s="1">
+        <v>3.5766946846591402E-13</v>
+      </c>
+      <c r="BA104" s="1">
+        <f t="shared" si="2"/>
+        <v>0.79923799960377584</v>
+      </c>
+      <c r="BB104" s="1">
+        <f t="shared" si="3"/>
+        <v>1.7058734022392665</v>
+      </c>
+    </row>
+    <row r="105" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A105" s="2"/>
+      <c r="B105" t="s">
+        <v>52</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1.0695735040804E-20</v>
+      </c>
+      <c r="D105" s="1">
+        <v>1.04239577324997E-19</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1.6473693402268801E-18</v>
+      </c>
+      <c r="F105" s="1">
+        <v>1.31487139397452E-18</v>
+      </c>
+      <c r="G105" s="1">
+        <v>5.6642005310514199E-19</v>
+      </c>
+      <c r="H105" s="1">
+        <v>2.9162813231658802E-19</v>
+      </c>
+      <c r="I105" s="1">
+        <v>1.06494049981009E-19</v>
+      </c>
+      <c r="J105" s="1">
+        <v>1.6267395538892701E-18</v>
+      </c>
+      <c r="K105" s="1">
+        <v>5.2492660941286896E-19</v>
+      </c>
+      <c r="L105" s="1">
+        <v>7.6756156969315394E-20</v>
+      </c>
+      <c r="M105" s="1">
+        <v>2.9918153825381301E-20</v>
+      </c>
+      <c r="N105" s="1">
+        <v>1.2642001870892499E-19</v>
+      </c>
+      <c r="O105" s="1">
+        <v>1.33486817005568E-19</v>
+      </c>
+      <c r="P105" s="1">
+        <v>3.3307356758611201E-19</v>
+      </c>
+      <c r="Q105" s="1">
+        <v>3.5314176493309501E-19</v>
+      </c>
+      <c r="R105" s="1">
+        <v>1.6586955660221799E-20</v>
+      </c>
+      <c r="S105" s="1">
+        <v>7.0213869142135595E-20</v>
+      </c>
+      <c r="T105" s="1">
+        <v>4.6349277649919198E-17</v>
+      </c>
+      <c r="U105" s="1">
+        <v>1.4122517663883E-19</v>
+      </c>
+      <c r="V105" s="1">
+        <v>2.9787174023391103E-20</v>
+      </c>
+      <c r="W105" s="1">
+        <v>3.5091685202561701E-21</v>
+      </c>
+      <c r="X105" s="1">
+        <v>4.7610573467450999E-20</v>
+      </c>
+      <c r="Y105" s="1">
+        <v>1.1512006269676299E-19</v>
+      </c>
+      <c r="Z105" s="1">
+        <v>1.5408159531933799E-19</v>
+      </c>
+      <c r="AA105" s="1">
+        <v>1.3220023135950901E-20</v>
+      </c>
+      <c r="AB105" s="1">
+        <v>3.1566723867168802E-21</v>
+      </c>
+      <c r="AC105" s="1">
+        <v>1.7953363173353201E-17</v>
+      </c>
+      <c r="AD105" s="1">
+        <v>5.6926171725428904E-20</v>
+      </c>
+      <c r="AE105" s="1">
+        <v>1.9340442926514198E-18</v>
+      </c>
+      <c r="AF105" s="1">
+        <v>1.37376817179419E-19</v>
+      </c>
+      <c r="AG105" s="1">
+        <v>4.6111264089416702E-19</v>
+      </c>
+      <c r="AH105" s="1">
+        <v>1.9372932180291599E-19</v>
+      </c>
+      <c r="AI105" s="1">
+        <v>1.8263538885573601E-19</v>
+      </c>
+      <c r="AJ105" s="1">
+        <v>5.9661798857202604E-19</v>
+      </c>
+      <c r="AK105" s="1">
+        <v>3.60139902549267E-19</v>
+      </c>
+      <c r="AL105" s="1">
+        <v>6.9095725305616595E-21</v>
+      </c>
+      <c r="AM105" s="1">
+        <v>1.65539890488566E-19</v>
+      </c>
+      <c r="AN105" s="1">
+        <v>5.5946696365357403E-19</v>
+      </c>
+      <c r="AO105" s="1">
+        <v>4.3242068423022198E-19</v>
+      </c>
+      <c r="AP105" s="1">
+        <v>1.3088601568050701E-20</v>
+      </c>
+      <c r="AQ105" s="1">
+        <v>4.6567536780997498E-19</v>
+      </c>
+      <c r="AR105" s="1">
+        <v>1.2225611684554801E-19</v>
+      </c>
+      <c r="AS105" s="1">
+        <v>1.9463864529601299E-19</v>
+      </c>
+      <c r="AT105" s="1">
+        <v>7.6359600161779902E-19</v>
+      </c>
+      <c r="AU105" s="1">
+        <v>5.5262499961467998E-18</v>
+      </c>
+      <c r="AV105" s="1">
+        <v>1.6305483842927501E-19</v>
+      </c>
+      <c r="AW105" s="1">
+        <v>1.06706913332286E-18</v>
+      </c>
+      <c r="AX105" s="1">
+        <v>4.7670432375575401E-20</v>
+      </c>
+      <c r="AY105" s="1">
+        <v>2.9398923479211499E-19</v>
+      </c>
+      <c r="AZ105" s="1">
+        <v>3.0097243925063402E-19</v>
+      </c>
+      <c r="BA105" s="1">
+        <f t="shared" si="2"/>
+        <v>1.7237702692230368E-18</v>
+      </c>
+      <c r="BB105" s="1">
+        <f t="shared" si="3"/>
+        <v>6.8817733079013645E-18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A106" s="2"/>
+      <c r="B106" t="s">
+        <v>53</v>
+      </c>
+      <c r="C106" s="1">
+        <v>107.278085966357</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1.88085926273059</v>
+      </c>
+      <c r="E106" s="1">
+        <v>3040.00990135245</v>
+      </c>
+      <c r="F106" s="1">
+        <v>14.8423249313827</v>
+      </c>
+      <c r="G106" s="1">
+        <v>81.528076309214796</v>
+      </c>
+      <c r="H106" s="1">
+        <v>259.51641154149701</v>
+      </c>
+      <c r="I106" s="1">
+        <v>3040.6562004543898</v>
+      </c>
+      <c r="J106" s="1">
+        <v>90028.797270140407</v>
+      </c>
+      <c r="K106" s="1">
+        <v>73.460313789151101</v>
+      </c>
+      <c r="L106" s="1">
+        <v>128.500718776425</v>
+      </c>
+      <c r="M106" s="1">
+        <v>95.682920402753794</v>
+      </c>
+      <c r="N106" s="1">
+        <v>25.421866425251999</v>
+      </c>
+      <c r="O106" s="1">
+        <v>28.949379194661098</v>
+      </c>
+      <c r="P106" s="1">
+        <v>24.875463970325001</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>25.7885412200818</v>
+      </c>
+      <c r="R106" s="1">
+        <v>77.197235857441598</v>
+      </c>
+      <c r="S106" s="1">
+        <v>77.982265003543503</v>
+      </c>
+      <c r="T106" s="1">
+        <v>76.649979067510301</v>
+      </c>
+      <c r="U106" s="1">
+        <v>24.128728061196401</v>
+      </c>
+      <c r="V106" s="1">
+        <v>90021.208995183697</v>
+      </c>
+      <c r="W106" s="1">
+        <v>11.3594364384132</v>
+      </c>
+      <c r="X106" s="1">
+        <v>24.860328420054799</v>
+      </c>
+      <c r="Y106" s="1">
+        <v>574.60668780510696</v>
+      </c>
+      <c r="Z106" s="1">
+        <v>28.021617125269799</v>
+      </c>
+      <c r="AA106" s="1">
+        <v>91.370591609761107</v>
+      </c>
+      <c r="AB106" s="1">
+        <v>3041.6244661036299</v>
+      </c>
+      <c r="AC106" s="1">
+        <v>90074.310970955004</v>
+      </c>
+      <c r="AD106" s="1">
+        <v>19.813819941314801</v>
+      </c>
+      <c r="AE106" s="1">
+        <v>24.625525370152602</v>
+      </c>
+      <c r="AF106" s="1">
+        <v>28.091426358557499</v>
+      </c>
+      <c r="AG106" s="1">
+        <v>24.2415516557584</v>
+      </c>
+      <c r="AH106" s="1">
+        <v>3041.8827106345898</v>
+      </c>
+      <c r="AI106" s="1">
+        <v>254.82308046290899</v>
+      </c>
+      <c r="AJ106" s="1">
+        <v>90025.090944899202</v>
+      </c>
+      <c r="AK106" s="1">
+        <v>68.543888859886906</v>
+      </c>
+      <c r="AL106" s="1">
+        <v>116.48995058407201</v>
+      </c>
+      <c r="AM106" s="1">
+        <v>122.767518341959</v>
+      </c>
+      <c r="AN106" s="1">
+        <v>73.712421332745095</v>
+      </c>
+      <c r="AO106" s="1">
+        <v>3029.67635318149</v>
+      </c>
+      <c r="AP106" s="1">
+        <v>630.05530060882404</v>
+      </c>
+      <c r="AQ106" s="1">
+        <v>3039.8692502359299</v>
+      </c>
+      <c r="AR106" s="1">
+        <v>76.155485219885307</v>
+      </c>
+      <c r="AS106" s="1">
+        <v>24.912166256586602</v>
+      </c>
+      <c r="AT106" s="1">
+        <v>3038.9405958318498</v>
+      </c>
+      <c r="AU106" s="1">
+        <v>21.0460297776599</v>
+      </c>
+      <c r="AV106" s="1">
+        <v>103.544505372575</v>
+      </c>
+      <c r="AW106" s="1">
+        <v>86.215245563031701</v>
+      </c>
+      <c r="AX106" s="1">
+        <v>100.29346319135701</v>
+      </c>
+      <c r="AY106" s="1">
+        <v>19.2845588826751</v>
+      </c>
+      <c r="AZ106" s="1">
+        <v>3041.7489622574899</v>
+      </c>
+      <c r="BA106" s="1">
+        <f t="shared" si="2"/>
+        <v>7762.2466878037631</v>
+      </c>
+      <c r="BB106" s="1">
+        <f t="shared" si="3"/>
+        <v>24285.465923578548</v>
+      </c>
+    </row>
+    <row r="107" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A107" s="2"/>
+      <c r="B107" t="s">
+        <v>54</v>
+      </c>
+      <c r="C107" s="1">
+        <v>20</v>
+      </c>
+      <c r="D107" s="1">
+        <v>30</v>
+      </c>
+      <c r="E107" s="1">
+        <v>2.2830387873266399E-14</v>
+      </c>
+      <c r="F107" s="1">
+        <v>5.2340182947574104E-15</v>
+      </c>
+      <c r="G107" s="1">
+        <v>10</v>
+      </c>
+      <c r="H107" s="1">
+        <v>10</v>
+      </c>
+      <c r="I107" s="1">
+        <v>2.9996496714984699E-15</v>
+      </c>
+      <c r="J107" s="1">
+        <v>10</v>
+      </c>
+      <c r="K107" s="1">
+        <v>1.2289187350826199E-14</v>
+      </c>
+      <c r="L107" s="1">
+        <v>9.2504643606075807E-15</v>
+      </c>
+      <c r="M107" s="1">
+        <v>5.7059198875807903E-15</v>
+      </c>
+      <c r="N107" s="1">
+        <v>8.1718987001762899E-14</v>
+      </c>
+      <c r="O107" s="1">
+        <v>10</v>
+      </c>
+      <c r="P107" s="1">
+        <v>9.3822103158828101E-15</v>
+      </c>
+      <c r="Q107" s="1">
+        <v>5.2756586370045099E-14</v>
+      </c>
+      <c r="R107" s="1">
+        <v>10</v>
+      </c>
+      <c r="S107" s="1">
+        <v>10</v>
+      </c>
+      <c r="T107" s="1">
+        <v>1.02381355524419E-14</v>
+      </c>
+      <c r="U107" s="1">
+        <v>1.41347130919591E-14</v>
+      </c>
+      <c r="V107" s="1">
+        <v>4.2645829007008602E-15</v>
+      </c>
+      <c r="W107" s="1">
+        <v>2.10344771024955E-14</v>
+      </c>
+      <c r="X107" s="1">
+        <v>6.1060012663583703E-15</v>
+      </c>
+      <c r="Y107" s="1">
+        <v>1.33543686277438E-14</v>
+      </c>
+      <c r="Z107" s="1">
+        <v>2.4799119216949001E-14</v>
+      </c>
+      <c r="AA107" s="1">
+        <v>30</v>
+      </c>
+      <c r="AB107" s="1">
+        <v>3.67677975147169E-14</v>
+      </c>
+      <c r="AC107" s="1">
+        <v>20</v>
+      </c>
+      <c r="AD107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF107" s="1">
+        <v>8.0499883383514195E-14</v>
+      </c>
+      <c r="AG107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AH107" s="1">
+        <v>2.1583131658168999E-14</v>
+      </c>
+      <c r="AI107" s="1">
+        <v>9.2641036843297902E-15</v>
+      </c>
+      <c r="AJ107" s="1">
+        <v>20</v>
+      </c>
+      <c r="AK107" s="1">
+        <v>1.0467695368201E-14</v>
+      </c>
+      <c r="AL107" s="1">
+        <v>2.7918936808635902E-14</v>
+      </c>
+      <c r="AM107" s="1">
+        <v>9.9976901801403598E-15</v>
+      </c>
+      <c r="AN107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AO107" s="1">
+        <v>1.0459157237150999E-14</v>
+      </c>
+      <c r="AP107" s="1">
+        <v>4.9473760529429303E-15</v>
+      </c>
+      <c r="AQ107" s="1">
+        <v>20</v>
+      </c>
+      <c r="AR107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AS107" s="1">
+        <v>1.6826277937932701E-15</v>
+      </c>
+      <c r="AT107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AU107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AV107" s="1">
+        <v>6.1205641374723099E-14</v>
+      </c>
+      <c r="AW107" s="1">
+        <v>6.2816417128942097E-15</v>
+      </c>
+      <c r="AX107" s="1">
+        <v>7.1080987287418496E-15</v>
+      </c>
+      <c r="AY107" s="1">
+        <v>10</v>
+      </c>
+      <c r="AZ107" s="1">
+        <v>4.10361330617018E-14</v>
+      </c>
+      <c r="BA107" s="1">
+        <f t="shared" si="2"/>
+        <v>5.6000000000000112</v>
+      </c>
+      <c r="BB107" s="1">
+        <f t="shared" si="3"/>
+        <v>8.0399004968967045</v>
+      </c>
+    </row>
+    <row r="108" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A108" s="2"/>
+      <c r="B108" t="s">
+        <v>55</v>
+      </c>
+      <c r="C108" s="1">
+        <v>4.2898477937247503E-40</v>
+      </c>
+      <c r="D108" s="1">
+        <v>3.0973857337675699E-36</v>
+      </c>
+      <c r="E108" s="1">
+        <v>1.16240829102001E-31</v>
+      </c>
+      <c r="F108" s="1">
+        <v>2.1010221076570602E-33</v>
+      </c>
+      <c r="G108" s="1">
+        <v>9.8850439821962597E-37</v>
+      </c>
+      <c r="H108" s="1">
+        <v>3.4831048765602702E-38</v>
+      </c>
+      <c r="I108" s="1">
+        <v>7.1742475479611001E-36</v>
+      </c>
+      <c r="J108" s="1">
+        <v>3.2929200262784001E-40</v>
+      </c>
+      <c r="K108" s="1">
+        <v>1.2941363138017499E-38</v>
+      </c>
+      <c r="L108" s="1">
+        <v>1.75423949363829E-37</v>
+      </c>
+      <c r="M108" s="1">
+        <v>2.89550728434293E-39</v>
+      </c>
+      <c r="N108" s="1">
+        <v>1.8628789032582499E-39</v>
+      </c>
+      <c r="O108" s="1">
+        <v>1.1887354953436901E-37</v>
+      </c>
+      <c r="P108" s="1">
+        <v>4.3099220120951802E-36</v>
+      </c>
+      <c r="Q108" s="1">
+        <v>3.5876097177205101E-32</v>
+      </c>
+      <c r="R108" s="1">
+        <v>1.1562469328265301E-35</v>
+      </c>
+      <c r="S108" s="1">
+        <v>3.1154667969289601E-40</v>
+      </c>
+      <c r="T108" s="1">
+        <v>2.7494027146096701E-36</v>
+      </c>
+      <c r="U108" s="1">
+        <v>1.23157153799205E-38</v>
+      </c>
+      <c r="V108" s="1">
+        <v>4.8419700185862102E-41</v>
+      </c>
+      <c r="W108" s="1">
+        <v>1.12106117768348E-34</v>
+      </c>
+      <c r="X108" s="1">
+        <v>9.88738641678451E-35</v>
+      </c>
+      <c r="Y108" s="1">
+        <v>3.3146448501764299E-37</v>
+      </c>
+      <c r="Z108" s="1">
+        <v>8.5193262062517906E-37</v>
+      </c>
+      <c r="AA108" s="1">
+        <v>8.1061099688794401E-35</v>
+      </c>
+      <c r="AB108" s="1">
+        <v>9.9724369232605701E-38</v>
+      </c>
+      <c r="AC108" s="1">
+        <v>1.8961795864061301E-34</v>
+      </c>
+      <c r="AD108" s="1">
+        <v>2.4635048739044602E-35</v>
+      </c>
+      <c r="AE108" s="1">
+        <v>1.3449757929535E-30</v>
+      </c>
+      <c r="AF108" s="1">
+        <v>8.9912818007028502E-38</v>
+      </c>
+      <c r="AG108" s="1">
+        <v>6.4588121684816704E-39</v>
+      </c>
+      <c r="AH108" s="1">
+        <v>1.25353582043323E-36</v>
+      </c>
+      <c r="AI108" s="1">
+        <v>1.0472142791861999E-33</v>
+      </c>
+      <c r="AJ108" s="1">
+        <v>1.55434141145522E-36</v>
+      </c>
+      <c r="AK108" s="1">
+        <v>2.2808553793969699E-39</v>
+      </c>
+      <c r="AL108" s="1">
+        <v>2.7062071463033599E-35</v>
+      </c>
+      <c r="AM108" s="1">
+        <v>4.58229482442821E-34</v>
+      </c>
+      <c r="AN108" s="1">
+        <v>1.2492352722864501E-34</v>
+      </c>
+      <c r="AO108" s="1">
+        <v>1.30517205443643E-33</v>
+      </c>
+      <c r="AP108" s="1">
+        <v>3.1817882557947098E-39</v>
+      </c>
+      <c r="AQ108" s="1">
+        <v>8.9043008639033299E-34</v>
+      </c>
+      <c r="AR108" s="1">
+        <v>2.6392693447640599E-40</v>
+      </c>
+      <c r="AS108" s="1">
+        <v>3.8115724810747997E-37</v>
+      </c>
+      <c r="AT108" s="1">
+        <v>1.9858473058570599E-38</v>
+      </c>
+      <c r="AU108" s="1">
+        <v>6.1918762666996203E-36</v>
+      </c>
+      <c r="AV108" s="1">
+        <v>3.1040144475240698E-33</v>
+      </c>
+      <c r="AW108" s="1">
+        <v>1.0968039878161001E-43</v>
+      </c>
+      <c r="AX108" s="1">
+        <v>9.0349635598013295E-40</v>
+      </c>
+      <c r="AY108" s="1">
+        <v>2.6469999307322301E-36</v>
+      </c>
+      <c r="AZ108" s="1">
+        <v>6.3637546542907096E-37</v>
+      </c>
+      <c r="BA108" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0134027876798544E-32</v>
+      </c>
+      <c r="BB108" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8859341774223188E-31</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A92:A99"/>
+    <mergeCell ref="A101:A108"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A20:A27"/>
+    <mergeCell ref="A29:A36"/>
+    <mergeCell ref="A38:A45"/>
     <mergeCell ref="A74:A81"/>
     <mergeCell ref="A83:A90"/>
     <mergeCell ref="A47:A54"/>
     <mergeCell ref="A56:A63"/>
     <mergeCell ref="A65:A72"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A38:A45"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add code of CLPSO & its data
</commit_message>
<xml_diff>
--- a/萝卜代码开会/PSOs+测试函数+仿真结果/PSO.xlsx
+++ b/萝卜代码开会/PSOs+测试函数+仿真结果/PSO.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001338E2-62B2-453F-892C-2E8972768374}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB1C4FA-25F7-43E1-9A52-5229B1F6E1AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
   <si>
     <t>基本PSO+Ackley</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,42 +76,6 @@
     <t>D=30
 N=80</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标准PSO+Ackley</t>
-  </si>
-  <si>
-    <t>标准PSO+Ackley</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标准PSO+Rastrigin</t>
-  </si>
-  <si>
-    <t>标准PSO+Rastrigin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标准PSO+Griewank</t>
-  </si>
-  <si>
-    <t>标准PSO+Griewank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>标准PSO+Alpine</t>
-  </si>
-  <si>
-    <t>标准PSO+Sphere</t>
-  </si>
-  <si>
-    <t>标准PSO+Rosenbrock</t>
-  </si>
-  <si>
-    <t>标准PSO+Schwefel</t>
-  </si>
-  <si>
-    <t>标准PSO+SDP</t>
   </si>
   <si>
     <t>D=30
@@ -214,6 +178,54 @@
   </si>
   <si>
     <t>BBPSO+SDP</t>
+  </si>
+  <si>
+    <t>GPSO+Ackley</t>
+  </si>
+  <si>
+    <t>GPSO+Rastrigin</t>
+  </si>
+  <si>
+    <t>GPSO+Griewank</t>
+  </si>
+  <si>
+    <t>GPSO+Alpine</t>
+  </si>
+  <si>
+    <t>GPSO+Sphere</t>
+  </si>
+  <si>
+    <t>GPSO+Rosenbrock</t>
+  </si>
+  <si>
+    <t>GPSO+Schwefel</t>
+  </si>
+  <si>
+    <t>GPSO+SDP</t>
+  </si>
+  <si>
+    <t>CLPSO+Ackley</t>
+  </si>
+  <si>
+    <t>CLPSO+Rastrigin</t>
+  </si>
+  <si>
+    <t>CLPSO+Griewank</t>
+  </si>
+  <si>
+    <t>CLPSO+Alpine</t>
+  </si>
+  <si>
+    <t>CLPSO+Sphere</t>
+  </si>
+  <si>
+    <t>CLPSO+Rosenbrock</t>
+  </si>
+  <si>
+    <t>CLPSO+Schwefel</t>
+  </si>
+  <si>
+    <t>CLPSO+SDP</t>
   </si>
 </sst>
 </file>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB108"/>
+  <dimension ref="A1:BB126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM89" workbookViewId="0">
-      <selection activeCell="AX105" sqref="AX105"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3353,7 +3365,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1">
         <v>4.4517378277161797</v>
@@ -3517,7 +3529,7 @@
     <row r="21" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1">
         <v>8.6134025495553797</v>
@@ -3681,7 +3693,7 @@
     <row r="22" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1">
         <v>0.396714405889873</v>
@@ -3845,7 +3857,7 @@
     <row r="23" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1">
         <v>0.74460071729645805</v>
@@ -4009,7 +4021,7 @@
     <row r="24" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1">
         <v>5.44498713386914</v>
@@ -4173,7 +4185,7 @@
     <row r="25" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1">
         <v>15.2525057254795</v>
@@ -4337,7 +4349,7 @@
     <row r="26" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C26" s="1">
         <v>0.60950146919100301</v>
@@ -4501,7 +4513,7 @@
     <row r="27" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1">
         <v>3.4192610092176298E-8</v>
@@ -4668,10 +4680,10 @@
     </row>
     <row r="29" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1">
         <v>4.1923712301748797</v>
@@ -4835,7 +4847,7 @@
     <row r="30" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1">
         <v>48.3411731400302</v>
@@ -4999,7 +5011,7 @@
     <row r="31" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1">
         <v>1.57033647982549</v>
@@ -5163,7 +5175,7 @@
     <row r="32" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1">
         <v>2.3932466200525102</v>
@@ -5327,7 +5339,7 @@
     <row r="33" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1">
         <v>46.213874129906898</v>
@@ -5491,7 +5503,7 @@
     <row r="34" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1">
         <v>425.97880809779502</v>
@@ -5655,7 +5667,7 @@
     <row r="35" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C35" s="1">
         <v>3.9520497228906102</v>
@@ -5819,7 +5831,7 @@
     <row r="36" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1">
         <v>6.0444841230930603E-9</v>
@@ -5989,7 +6001,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1">
         <v>2.7959853017872001</v>
@@ -6153,7 +6165,7 @@
     <row r="39" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C39" s="1">
         <v>13.960159193973</v>
@@ -6317,7 +6329,7 @@
     <row r="40" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C40" s="1">
         <v>0.22240723611150501</v>
@@ -6481,7 +6493,7 @@
     <row r="41" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1">
         <v>3.6595372252924099E-2</v>
@@ -6645,7 +6657,7 @@
     <row r="42" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1">
         <v>7.7939287304225205E-4</v>
@@ -6809,7 +6821,7 @@
     <row r="43" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C43" s="1">
         <v>8.90570915970555</v>
@@ -6973,7 +6985,7 @@
     <row r="44" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C44" s="1">
         <v>0.105042101379468</v>
@@ -7137,7 +7149,7 @@
     <row r="45" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C45" s="1">
         <v>2.5827972614623598E-9</v>
@@ -7307,7 +7319,7 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1">
         <v>5.2650937945424001</v>
@@ -7471,7 +7483,7 @@
     <row r="48" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C48" s="1">
         <v>39.9609523384959</v>
@@ -7635,7 +7647,7 @@
     <row r="49" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C49" s="1">
         <v>0.33162308795579398</v>
@@ -7799,7 +7811,7 @@
     <row r="50" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C50" s="1">
         <v>0.19654782432144299</v>
@@ -7963,7 +7975,7 @@
     <row r="51" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C51" s="1">
         <v>1.32198910270494</v>
@@ -8127,7 +8139,7 @@
     <row r="52" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C52" s="1">
         <v>141.04690051403301</v>
@@ -8291,7 +8303,7 @@
     <row r="53" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C53" s="1">
         <v>6.3340565861841904</v>
@@ -8455,7 +8467,7 @@
     <row r="54" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C54" s="1">
         <v>4.0766092221677597E-11</v>
@@ -8625,7 +8637,7 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C56" s="1">
         <v>2.3213700791040099</v>
@@ -8789,7 +8801,7 @@
     <row r="57" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C57" s="1">
         <v>6.1744440650644297</v>
@@ -8953,7 +8965,7 @@
     <row r="58" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C58" s="1">
         <v>0.33415843240811799</v>
@@ -9117,7 +9129,7 @@
     <row r="59" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C59" s="1">
         <v>4.0080005481802402E-3</v>
@@ -9281,7 +9293,7 @@
     <row r="60" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C60" s="1">
         <v>1.05185961420038</v>
@@ -9445,7 +9457,7 @@
     <row r="61" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C61" s="1">
         <v>24.871584017508599</v>
@@ -9609,7 +9621,7 @@
     <row r="62" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C62" s="1">
         <v>1.30710379048676</v>
@@ -9773,7 +9785,7 @@
     <row r="63" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C63" s="1">
         <v>1.53768489786924E-7</v>
@@ -9943,7 +9955,7 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C65" s="1">
         <v>3.5500388072209499</v>
@@ -10107,7 +10119,7 @@
     <row r="66" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C66" s="1">
         <v>40.688620931617898</v>
@@ -10271,7 +10283,7 @@
     <row r="67" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C67" s="1">
         <v>1.0688470765328599</v>
@@ -10424,18 +10436,18 @@
         <v>1.13028885427138</v>
       </c>
       <c r="BA67" s="1">
-        <f t="shared" ref="BA67:BA108" si="2">AVERAGE(C67:AZ67)</f>
+        <f t="shared" ref="BA67:BA126" si="2">AVERAGE(C67:AZ67)</f>
         <v>1.3061262637510567</v>
       </c>
       <c r="BB67" s="1">
-        <f t="shared" ref="BB67:BB108" si="3">STDEVP(C67:AZ67)</f>
+        <f t="shared" ref="BB67:BB126" si="3">STDEVP(C67:AZ67)</f>
         <v>0.13151924759816777</v>
       </c>
     </row>
     <row r="68" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C68" s="1">
         <v>1.46632520330445</v>
@@ -10599,7 +10611,7 @@
     <row r="69" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C69" s="1">
         <v>16.4320894863828</v>
@@ -10763,7 +10775,7 @@
     <row r="70" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C70" s="1">
         <v>486.97166559187298</v>
@@ -10927,7 +10939,7 @@
     <row r="71" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C71" s="1">
         <v>7.5524165169136701</v>
@@ -11091,7 +11103,7 @@
     <row r="72" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C72" s="1">
         <v>1.6696641203835501E-13</v>
@@ -11261,7 +11273,7 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C74" s="1">
         <v>2.5831826254250698</v>
@@ -11425,7 +11437,7 @@
     <row r="75" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C75" s="1">
         <v>7.0050929443885197</v>
@@ -11589,7 +11601,7 @@
     <row r="76" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1">
         <v>0.411009166388558</v>
@@ -11753,7 +11765,7 @@
     <row r="77" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C77" s="1">
         <v>0.17014354046579599</v>
@@ -11917,7 +11929,7 @@
     <row r="78" spans="1:54" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C78" s="1">
         <v>1.0999107361464699</v>
@@ -12081,7 +12093,7 @@
     <row r="79" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C79" s="1">
         <v>35.5754489305384</v>
@@ -12245,7 +12257,7 @@
     <row r="80" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C80" s="1">
         <v>0.52457791511003904</v>
@@ -12409,7 +12421,7 @@
     <row r="81" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C81" s="1">
         <v>1.3438704393310899E-10</v>
@@ -12579,7 +12591,7 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C83" s="1">
         <v>5.0957078604647403</v>
@@ -12743,7 +12755,7 @@
     <row r="84" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C84" s="1">
         <v>25.035990058174502</v>
@@ -12907,7 +12919,7 @@
     <row r="85" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C85" s="1">
         <v>1.01605792426782</v>
@@ -13071,7 +13083,7 @@
     <row r="86" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C86" s="1">
         <v>0.34859307524675398</v>
@@ -13235,7 +13247,7 @@
     <row r="87" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C87" s="1">
         <v>3.3988264777243402</v>
@@ -13399,7 +13411,7 @@
     <row r="88" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C88" s="1">
         <v>106.75796340260599</v>
@@ -13563,7 +13575,7 @@
     <row r="89" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C89" s="1">
         <v>1.83829229708576</v>
@@ -13727,7 +13739,7 @@
     <row r="90" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C90" s="1">
         <v>7.4181705235445699E-17</v>
@@ -13897,7 +13909,7 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C92" s="1">
         <v>3.5527136788005001E-15</v>
@@ -14061,7 +14073,7 @@
     <row r="93" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C93" s="1">
         <v>13.9294116858488</v>
@@ -14225,7 +14237,7 @@
     <row r="94" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C94" s="1">
         <v>8.6244538392177897E-2</v>
@@ -14389,7 +14401,7 @@
     <row r="95" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C95" s="1">
         <v>2.72698530423554E-15</v>
@@ -14553,7 +14565,7 @@
     <row r="96" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C96" s="1">
         <v>2.9283202285055101E-73</v>
@@ -14717,7 +14729,7 @@
     <row r="97" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C97" s="1">
         <v>0.160738698826772</v>
@@ -14881,7 +14893,7 @@
     <row r="98" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C98" s="1">
         <v>1.10983467393134E-44</v>
@@ -15045,7 +15057,7 @@
     <row r="99" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C99" s="1">
         <v>1.7125425911264801E-136</v>
@@ -15265,7 +15277,7 @@
         <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C101" s="1">
         <v>2.3858603981352598E-10</v>
@@ -15429,7 +15441,7 @@
     <row r="102" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C102" s="1">
         <v>40.793265879376897</v>
@@ -15593,7 +15605,7 @@
     <row r="103" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C103" s="1">
         <v>0</v>
@@ -15757,7 +15769,7 @@
     <row r="104" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C104" s="1">
         <v>4.4402111088937399</v>
@@ -15921,7 +15933,7 @@
     <row r="105" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C105" s="1">
         <v>1.0695735040804E-20</v>
@@ -16085,7 +16097,7 @@
     <row r="106" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C106" s="1">
         <v>107.278085966357</v>
@@ -16249,7 +16261,7 @@
     <row r="107" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C107" s="1">
         <v>20</v>
@@ -16413,7 +16425,7 @@
     <row r="108" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C108" s="1">
         <v>4.2898477937247503E-40</v>
@@ -16574,8 +16586,2696 @@
         <v>1.8859341774223188E-31</v>
       </c>
     </row>
+    <row r="109" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="BA109" s="1"/>
+      <c r="BB109" s="1"/>
+    </row>
+    <row r="110" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B110" t="s">
+        <v>53</v>
+      </c>
+      <c r="C110" s="1">
+        <v>11.1659840490088</v>
+      </c>
+      <c r="D110" s="1">
+        <v>14.092124293787901</v>
+      </c>
+      <c r="E110" s="1">
+        <v>10.7283915499745</v>
+      </c>
+      <c r="F110" s="1">
+        <v>6.6210802437324201</v>
+      </c>
+      <c r="G110" s="1">
+        <v>8.2212930404459001</v>
+      </c>
+      <c r="H110" s="1">
+        <v>10.8971062278952</v>
+      </c>
+      <c r="I110" s="1">
+        <v>8.2866705143799404</v>
+      </c>
+      <c r="J110" s="1">
+        <v>12.3099432259036</v>
+      </c>
+      <c r="K110" s="1">
+        <v>9.1450822168785404</v>
+      </c>
+      <c r="L110" s="1">
+        <v>8.9423798666882899</v>
+      </c>
+      <c r="M110" s="1">
+        <v>8.5799957632035202</v>
+      </c>
+      <c r="N110" s="1">
+        <v>11.1710112338423</v>
+      </c>
+      <c r="O110" s="1">
+        <v>6.5784157066724003</v>
+      </c>
+      <c r="P110" s="1">
+        <v>10.5209681419483</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>13.3021667226828</v>
+      </c>
+      <c r="R110" s="1">
+        <v>11.4485646806523</v>
+      </c>
+      <c r="S110" s="1">
+        <v>12.859757209588199</v>
+      </c>
+      <c r="T110" s="1">
+        <v>7.0134866908119902</v>
+      </c>
+      <c r="U110" s="1">
+        <v>13.172628228808</v>
+      </c>
+      <c r="V110" s="1">
+        <v>12.232285374290299</v>
+      </c>
+      <c r="W110" s="1">
+        <v>11.4469675833754</v>
+      </c>
+      <c r="X110" s="1">
+        <v>7.2881724505316496</v>
+      </c>
+      <c r="Y110" s="1">
+        <v>13.2313649891927</v>
+      </c>
+      <c r="Z110" s="1">
+        <v>8.6301585097711495</v>
+      </c>
+      <c r="AA110" s="1">
+        <v>3.9031479105414699</v>
+      </c>
+      <c r="AB110" s="1">
+        <v>13.0210100843448</v>
+      </c>
+      <c r="AC110" s="1">
+        <v>8.82689578365712</v>
+      </c>
+      <c r="AD110" s="1">
+        <v>12.4762130625193</v>
+      </c>
+      <c r="AE110" s="1">
+        <v>9.1203919807411005</v>
+      </c>
+      <c r="AF110" s="1">
+        <v>9.9838749336087194</v>
+      </c>
+      <c r="AG110" s="1">
+        <v>9.1724439697159301</v>
+      </c>
+      <c r="AH110" s="1">
+        <v>12.9091880695982</v>
+      </c>
+      <c r="AI110" s="1">
+        <v>9.9231156288300895</v>
+      </c>
+      <c r="AJ110" s="1">
+        <v>14.7535128005969</v>
+      </c>
+      <c r="AK110" s="1">
+        <v>13.929697484320201</v>
+      </c>
+      <c r="AL110" s="1">
+        <v>10.0259958186017</v>
+      </c>
+      <c r="AM110" s="1">
+        <v>6.7147959110806896</v>
+      </c>
+      <c r="AN110" s="1">
+        <v>14.435456861700599</v>
+      </c>
+      <c r="AO110" s="1">
+        <v>7.6487983720788399</v>
+      </c>
+      <c r="AP110" s="1">
+        <v>10.774827353594</v>
+      </c>
+      <c r="AQ110" s="1">
+        <v>15.371918881439999</v>
+      </c>
+      <c r="AR110" s="1">
+        <v>9.0422679340883896</v>
+      </c>
+      <c r="AS110" s="1">
+        <v>10.3145239874532</v>
+      </c>
+      <c r="AT110" s="1">
+        <v>11.115909564833499</v>
+      </c>
+      <c r="AU110" s="1">
+        <v>7.1096612606356802</v>
+      </c>
+      <c r="AV110" s="1">
+        <v>12.0269269035735</v>
+      </c>
+      <c r="AW110" s="1">
+        <v>6.5924903990693702</v>
+      </c>
+      <c r="AX110" s="1">
+        <v>9.2654726013753308</v>
+      </c>
+      <c r="AY110" s="1">
+        <v>9.97233970657736</v>
+      </c>
+      <c r="AZ110" s="1">
+        <v>11.3670985405516</v>
+      </c>
+      <c r="BA110" s="1">
+        <f t="shared" si="2"/>
+        <v>10.353679486383873</v>
+      </c>
+      <c r="BB110" s="1">
+        <f t="shared" si="3"/>
+        <v>2.514509305375229</v>
+      </c>
+    </row>
+    <row r="111" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A111" s="2"/>
+      <c r="B111" t="s">
+        <v>54</v>
+      </c>
+      <c r="C111" s="1">
+        <v>10.4244005107187</v>
+      </c>
+      <c r="D111" s="1">
+        <v>12.9835943397451</v>
+      </c>
+      <c r="E111" s="1">
+        <v>15.853978079704699</v>
+      </c>
+      <c r="F111" s="1">
+        <v>5.0680198479290999</v>
+      </c>
+      <c r="G111" s="1">
+        <v>10.5179289870829</v>
+      </c>
+      <c r="H111" s="1">
+        <v>9.1264195480504302</v>
+      </c>
+      <c r="I111" s="1">
+        <v>21.009586705194199</v>
+      </c>
+      <c r="J111" s="1">
+        <v>15.725954609007401</v>
+      </c>
+      <c r="K111" s="1">
+        <v>12.1491818129932</v>
+      </c>
+      <c r="L111" s="1">
+        <v>9.4510459427314704</v>
+      </c>
+      <c r="M111" s="1">
+        <v>10.930840895540101</v>
+      </c>
+      <c r="N111" s="1">
+        <v>17.323167447637299</v>
+      </c>
+      <c r="O111" s="1">
+        <v>7.2644595485592598</v>
+      </c>
+      <c r="P111" s="1">
+        <v>13.332868396364301</v>
+      </c>
+      <c r="Q111" s="1">
+        <v>3.8097877266352498</v>
+      </c>
+      <c r="R111" s="1">
+        <v>8.7577642442164105</v>
+      </c>
+      <c r="S111" s="1">
+        <v>8.4193947435267003</v>
+      </c>
+      <c r="T111" s="1">
+        <v>10.9344050449112</v>
+      </c>
+      <c r="U111" s="1">
+        <v>9.8000854817101892</v>
+      </c>
+      <c r="V111" s="1">
+        <v>11.1807617671038</v>
+      </c>
+      <c r="W111" s="1">
+        <v>6.9627161741113897</v>
+      </c>
+      <c r="X111" s="1">
+        <v>10.693397006074999</v>
+      </c>
+      <c r="Y111" s="1">
+        <v>4.4484703887431802</v>
+      </c>
+      <c r="Z111" s="1">
+        <v>9.2815915601537498</v>
+      </c>
+      <c r="AA111" s="1">
+        <v>6.6287702174074896</v>
+      </c>
+      <c r="AB111" s="1">
+        <v>5.7250729969000203</v>
+      </c>
+      <c r="AC111" s="1">
+        <v>5.7477446647932799</v>
+      </c>
+      <c r="AD111" s="1">
+        <v>3.2753229721515398</v>
+      </c>
+      <c r="AE111" s="1">
+        <v>12.5605313646452</v>
+      </c>
+      <c r="AF111" s="1">
+        <v>5.0800601696277896</v>
+      </c>
+      <c r="AG111" s="1">
+        <v>9.9979842132137495</v>
+      </c>
+      <c r="AH111" s="1">
+        <v>7.8241730258023203</v>
+      </c>
+      <c r="AI111" s="1">
+        <v>19.2922438658697</v>
+      </c>
+      <c r="AJ111" s="1">
+        <v>9.4928598656829095</v>
+      </c>
+      <c r="AK111" s="1">
+        <v>6.2237023811264001</v>
+      </c>
+      <c r="AL111" s="1">
+        <v>14.3498667926468</v>
+      </c>
+      <c r="AM111" s="1">
+        <v>13.5782438777505</v>
+      </c>
+      <c r="AN111" s="1">
+        <v>17.043999968338898</v>
+      </c>
+      <c r="AO111" s="1">
+        <v>6.1776930594457502</v>
+      </c>
+      <c r="AP111" s="1">
+        <v>8.73282084151875</v>
+      </c>
+      <c r="AQ111" s="1">
+        <v>14.0149511044959</v>
+      </c>
+      <c r="AR111" s="1">
+        <v>12.744805652076099</v>
+      </c>
+      <c r="AS111" s="1">
+        <v>7.2708802079919401</v>
+      </c>
+      <c r="AT111" s="1">
+        <v>12.4860305622148</v>
+      </c>
+      <c r="AU111" s="1">
+        <v>10.231911352062699</v>
+      </c>
+      <c r="AV111" s="1">
+        <v>5.1503751252359304</v>
+      </c>
+      <c r="AW111" s="1">
+        <v>9.3733613830786808</v>
+      </c>
+      <c r="AX111" s="1">
+        <v>11.386085678300301</v>
+      </c>
+      <c r="AY111" s="1">
+        <v>8.4386769640943804</v>
+      </c>
+      <c r="AZ111" s="1">
+        <v>14.3827620321052</v>
+      </c>
+      <c r="BA111" s="1">
+        <f t="shared" si="2"/>
+        <v>10.25321502294044</v>
+      </c>
+      <c r="BB111" s="1">
+        <f t="shared" si="3"/>
+        <v>3.9872073754264594</v>
+      </c>
+    </row>
+    <row r="112" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A112" s="2"/>
+      <c r="B112" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112" s="1">
+        <v>48.8077762095201</v>
+      </c>
+      <c r="D112" s="1">
+        <v>53.949442371959897</v>
+      </c>
+      <c r="E112" s="1">
+        <v>46.4689518202863</v>
+      </c>
+      <c r="F112" s="1">
+        <v>73.820323358248601</v>
+      </c>
+      <c r="G112" s="1">
+        <v>46.448802234308801</v>
+      </c>
+      <c r="H112" s="1">
+        <v>92.138175808688302</v>
+      </c>
+      <c r="I112" s="1">
+        <v>35.0200500842124</v>
+      </c>
+      <c r="J112" s="1">
+        <v>43.979755999971204</v>
+      </c>
+      <c r="K112" s="1">
+        <v>82.647920640707</v>
+      </c>
+      <c r="L112" s="1">
+        <v>26.2863343233305</v>
+      </c>
+      <c r="M112" s="1">
+        <v>58.040490630495199</v>
+      </c>
+      <c r="N112" s="1">
+        <v>52.930956601829401</v>
+      </c>
+      <c r="O112" s="1">
+        <v>72.327057749401902</v>
+      </c>
+      <c r="P112" s="1">
+        <v>53.0889651450278</v>
+      </c>
+      <c r="Q112" s="1">
+        <v>55.6319381341048</v>
+      </c>
+      <c r="R112" s="1">
+        <v>74.205799056374303</v>
+      </c>
+      <c r="S112" s="1">
+        <v>65.463137117436105</v>
+      </c>
+      <c r="T112" s="1">
+        <v>52.883495264327998</v>
+      </c>
+      <c r="U112" s="1">
+        <v>53.858980403587097</v>
+      </c>
+      <c r="V112" s="1">
+        <v>75.234628351490898</v>
+      </c>
+      <c r="W112" s="1">
+        <v>73.056422888216503</v>
+      </c>
+      <c r="X112" s="1">
+        <v>67.775173022998402</v>
+      </c>
+      <c r="Y112" s="1">
+        <v>37.153194242105798</v>
+      </c>
+      <c r="Z112" s="1">
+        <v>60.145096033352303</v>
+      </c>
+      <c r="AA112" s="1">
+        <v>70.260091840216802</v>
+      </c>
+      <c r="AB112" s="1">
+        <v>42.277493979554002</v>
+      </c>
+      <c r="AC112" s="1">
+        <v>97.472729180369399</v>
+      </c>
+      <c r="AD112" s="1">
+        <v>74.842805862525097</v>
+      </c>
+      <c r="AE112" s="1">
+        <v>60.1287760388687</v>
+      </c>
+      <c r="AF112" s="1">
+        <v>117.09030402534501</v>
+      </c>
+      <c r="AG112" s="1">
+        <v>83.188759929249798</v>
+      </c>
+      <c r="AH112" s="1">
+        <v>49.882718481396502</v>
+      </c>
+      <c r="AI112" s="1">
+        <v>40.7408025899446</v>
+      </c>
+      <c r="AJ112" s="1">
+        <v>66.312959282501495</v>
+      </c>
+      <c r="AK112" s="1">
+        <v>37.992747442933002</v>
+      </c>
+      <c r="AL112" s="1">
+        <v>37.364756271367902</v>
+      </c>
+      <c r="AM112" s="1">
+        <v>67.417087590841206</v>
+      </c>
+      <c r="AN112" s="1">
+        <v>64.341284477755195</v>
+      </c>
+      <c r="AO112" s="1">
+        <v>71.276991557030598</v>
+      </c>
+      <c r="AP112" s="1">
+        <v>49.479257769585899</v>
+      </c>
+      <c r="AQ112" s="1">
+        <v>43.286733626475197</v>
+      </c>
+      <c r="AR112" s="1">
+        <v>48.829205435156801</v>
+      </c>
+      <c r="AS112" s="1">
+        <v>68.586148243234803</v>
+      </c>
+      <c r="AT112" s="1">
+        <v>43.9099425713678</v>
+      </c>
+      <c r="AU112" s="1">
+        <v>60.859746029362</v>
+      </c>
+      <c r="AV112" s="1">
+        <v>39.867062251609099</v>
+      </c>
+      <c r="AW112" s="1">
+        <v>37.0535104644702</v>
+      </c>
+      <c r="AX112" s="1">
+        <v>45.086840704294502</v>
+      </c>
+      <c r="AY112" s="1">
+        <v>78.675937703387007</v>
+      </c>
+      <c r="AZ112" s="1">
+        <v>74.054948463687495</v>
+      </c>
+      <c r="BA112" s="1">
+        <f t="shared" si="2"/>
+        <v>59.432850186090235</v>
+      </c>
+      <c r="BB112" s="1">
+        <f t="shared" si="3"/>
+        <v>17.857608130353473</v>
+      </c>
+    </row>
+    <row r="113" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A113" s="2"/>
+      <c r="B113" t="s">
+        <v>56</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.19181027585118801</v>
+      </c>
+      <c r="D113" s="1">
+        <v>0.154137218153267</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0.12851917080331801</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0.245820845156759</v>
+      </c>
+      <c r="G113" s="1">
+        <v>0.29478660794272299</v>
+      </c>
+      <c r="H113" s="1">
+        <v>0.12188220476315199</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0.96857565305738003</v>
+      </c>
+      <c r="J113" s="1">
+        <v>0.33947528373569802</v>
+      </c>
+      <c r="K113" s="1">
+        <v>0.75112426634799401</v>
+      </c>
+      <c r="L113" s="1">
+        <v>0.242347750479359</v>
+      </c>
+      <c r="M113" s="1">
+        <v>0.30815734793213201</v>
+      </c>
+      <c r="N113" s="1">
+        <v>0.10678934542390101</v>
+      </c>
+      <c r="O113" s="1">
+        <v>0.12986882322819901</v>
+      </c>
+      <c r="P113" s="1">
+        <v>0.139363572450728</v>
+      </c>
+      <c r="Q113" s="1">
+        <v>0.36697206277558198</v>
+      </c>
+      <c r="R113" s="1">
+        <v>0.209691076493875</v>
+      </c>
+      <c r="S113" s="1">
+        <v>0.27399971569598103</v>
+      </c>
+      <c r="T113" s="1">
+        <v>0.24884416269982301</v>
+      </c>
+      <c r="U113" s="1">
+        <v>6.7330176928023802E-2</v>
+      </c>
+      <c r="V113" s="1">
+        <v>0.53691312344365405</v>
+      </c>
+      <c r="W113" s="1">
+        <v>0.39996692058322703</v>
+      </c>
+      <c r="X113" s="1">
+        <v>2.81697883440176E-2</v>
+      </c>
+      <c r="Y113" s="1">
+        <v>0.19768064725565301</v>
+      </c>
+      <c r="Z113" s="1">
+        <v>0.46968908700971801</v>
+      </c>
+      <c r="AA113" s="1">
+        <v>0.119113084284139</v>
+      </c>
+      <c r="AB113" s="1">
+        <v>0.42265828737539801</v>
+      </c>
+      <c r="AC113" s="1">
+        <v>0.27932652362881499</v>
+      </c>
+      <c r="AD113" s="1">
+        <v>0.89104592903673996</v>
+      </c>
+      <c r="AE113" s="1">
+        <v>0.192518854891986</v>
+      </c>
+      <c r="AF113" s="1">
+        <v>0.56421861159324804</v>
+      </c>
+      <c r="AG113" s="1">
+        <v>5.9908581895292398E-2</v>
+      </c>
+      <c r="AH113" s="1">
+        <v>0.44822306883995999</v>
+      </c>
+      <c r="AI113" s="1">
+        <v>0.33335500467637103</v>
+      </c>
+      <c r="AJ113" s="1">
+        <v>0.26004903286883801</v>
+      </c>
+      <c r="AK113" s="1">
+        <v>0.131032101226944</v>
+      </c>
+      <c r="AL113" s="1">
+        <v>1.1262658365361999</v>
+      </c>
+      <c r="AM113" s="1">
+        <v>8.8379478971635894E-2</v>
+      </c>
+      <c r="AN113" s="1">
+        <v>0.28085585260628698</v>
+      </c>
+      <c r="AO113" s="1">
+        <v>0.11592670967551499</v>
+      </c>
+      <c r="AP113" s="1">
+        <v>0.123860920219485</v>
+      </c>
+      <c r="AQ113" s="1">
+        <v>0.26743537880943102</v>
+      </c>
+      <c r="AR113" s="1">
+        <v>0.31247073957726101</v>
+      </c>
+      <c r="AS113" s="1">
+        <v>6.7922860705491403E-2</v>
+      </c>
+      <c r="AT113" s="1">
+        <v>0.46217200347741799</v>
+      </c>
+      <c r="AU113" s="1">
+        <v>0.13310069757947299</v>
+      </c>
+      <c r="AV113" s="1">
+        <v>0.90363804638405898</v>
+      </c>
+      <c r="AW113" s="1">
+        <v>4.73658527662957E-2</v>
+      </c>
+      <c r="AX113" s="1">
+        <v>0.118779306975525</v>
+      </c>
+      <c r="AY113" s="1">
+        <v>0.14304735518608799</v>
+      </c>
+      <c r="AZ113" s="1">
+        <v>0.242407103434995</v>
+      </c>
+      <c r="BA113" s="1">
+        <f t="shared" si="2"/>
+        <v>0.30113984699556495</v>
+      </c>
+      <c r="BB113" s="1">
+        <f t="shared" si="3"/>
+        <v>0.24797794263341652</v>
+      </c>
+    </row>
+    <row r="114" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A114" s="2"/>
+      <c r="B114" t="s">
+        <v>57</v>
+      </c>
+      <c r="C114" s="1">
+        <v>724.72639516370396</v>
+      </c>
+      <c r="D114" s="1">
+        <v>649.35908897032505</v>
+      </c>
+      <c r="E114" s="1">
+        <v>724.55469449452596</v>
+      </c>
+      <c r="F114" s="1">
+        <v>1191.03190255972</v>
+      </c>
+      <c r="G114" s="1">
+        <v>82.766788994125605</v>
+      </c>
+      <c r="H114" s="1">
+        <v>2395.8202088686298</v>
+      </c>
+      <c r="I114" s="1">
+        <v>909.42409439345397</v>
+      </c>
+      <c r="J114" s="1">
+        <v>1587.5571980458101</v>
+      </c>
+      <c r="K114" s="1">
+        <v>406.838813880288</v>
+      </c>
+      <c r="L114" s="1">
+        <v>1853.51310679528</v>
+      </c>
+      <c r="M114" s="1">
+        <v>825.18599698268804</v>
+      </c>
+      <c r="N114" s="1">
+        <v>1335.63490028623</v>
+      </c>
+      <c r="O114" s="1">
+        <v>1151.7270457378399</v>
+      </c>
+      <c r="P114" s="1">
+        <v>2932.0991125109099</v>
+      </c>
+      <c r="Q114" s="1">
+        <v>429.19654772491702</v>
+      </c>
+      <c r="R114" s="1">
+        <v>1041.87618139084</v>
+      </c>
+      <c r="S114" s="1">
+        <v>1010.31664053942</v>
+      </c>
+      <c r="T114" s="1">
+        <v>726.38968181802204</v>
+      </c>
+      <c r="U114" s="1">
+        <v>411.92278971078701</v>
+      </c>
+      <c r="V114" s="1">
+        <v>2278.1899413167898</v>
+      </c>
+      <c r="W114" s="1">
+        <v>716.97889486274801</v>
+      </c>
+      <c r="X114" s="1">
+        <v>1079.55214341603</v>
+      </c>
+      <c r="Y114" s="1">
+        <v>938.78656816602199</v>
+      </c>
+      <c r="Z114" s="1">
+        <v>725.58504490651296</v>
+      </c>
+      <c r="AA114" s="1">
+        <v>627.92435850871402</v>
+      </c>
+      <c r="AB114" s="1">
+        <v>3504.5758144751198</v>
+      </c>
+      <c r="AC114" s="1">
+        <v>1151.1427199058301</v>
+      </c>
+      <c r="AD114" s="1">
+        <v>1056.0414894585299</v>
+      </c>
+      <c r="AE114" s="1">
+        <v>409.02083261783599</v>
+      </c>
+      <c r="AF114" s="1">
+        <v>641.61119808090996</v>
+      </c>
+      <c r="AG114" s="1">
+        <v>326.01076138362203</v>
+      </c>
+      <c r="AH114" s="1">
+        <v>1096.8654722516001</v>
+      </c>
+      <c r="AI114" s="1">
+        <v>326.75656109065</v>
+      </c>
+      <c r="AJ114" s="1">
+        <v>1127.3723561015299</v>
+      </c>
+      <c r="AK114" s="1">
+        <v>852.96746566015099</v>
+      </c>
+      <c r="AL114" s="1">
+        <v>1129.8533139976601</v>
+      </c>
+      <c r="AM114" s="1">
+        <v>1539.3588398202101</v>
+      </c>
+      <c r="AN114" s="1">
+        <v>962.957386613891</v>
+      </c>
+      <c r="AO114" s="1">
+        <v>2909.9734259152601</v>
+      </c>
+      <c r="AP114" s="1">
+        <v>648.113725208083</v>
+      </c>
+      <c r="AQ114" s="1">
+        <v>949.39155227282697</v>
+      </c>
+      <c r="AR114" s="1">
+        <v>1646.7698229668799</v>
+      </c>
+      <c r="AS114" s="1">
+        <v>2536.9137885462201</v>
+      </c>
+      <c r="AT114" s="1">
+        <v>424.72816554091003</v>
+      </c>
+      <c r="AU114" s="1">
+        <v>459.18374854654297</v>
+      </c>
+      <c r="AV114" s="1">
+        <v>1334.5150177529499</v>
+      </c>
+      <c r="AW114" s="1">
+        <v>510.29746661718002</v>
+      </c>
+      <c r="AX114" s="1">
+        <v>271.76590706723101</v>
+      </c>
+      <c r="AY114" s="1">
+        <v>696.82462539719302</v>
+      </c>
+      <c r="AZ114" s="1">
+        <v>631.71431211064305</v>
+      </c>
+      <c r="BA114" s="1">
+        <f t="shared" si="2"/>
+        <v>1078.0336781888757</v>
+      </c>
+      <c r="BB114" s="1">
+        <f t="shared" si="3"/>
+        <v>736.79824002545377</v>
+      </c>
+    </row>
+    <row r="115" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A115" s="2"/>
+      <c r="B115" t="s">
+        <v>58</v>
+      </c>
+      <c r="C115" s="1">
+        <v>9454.2270668542405</v>
+      </c>
+      <c r="D115" s="1">
+        <v>18163.7209680581</v>
+      </c>
+      <c r="E115" s="1">
+        <v>406517.29926150601</v>
+      </c>
+      <c r="F115" s="1">
+        <v>126094.551688608</v>
+      </c>
+      <c r="G115" s="1">
+        <v>164357.00610745899</v>
+      </c>
+      <c r="H115" s="1">
+        <v>10141.574158164</v>
+      </c>
+      <c r="I115" s="1">
+        <v>46516.339381067002</v>
+      </c>
+      <c r="J115" s="1">
+        <v>231817.13501607999</v>
+      </c>
+      <c r="K115" s="1">
+        <v>66436.172860095205</v>
+      </c>
+      <c r="L115" s="1">
+        <v>9845.9396144136899</v>
+      </c>
+      <c r="M115" s="1">
+        <v>1950.05060003633</v>
+      </c>
+      <c r="N115" s="1">
+        <v>6901.2830886203101</v>
+      </c>
+      <c r="O115" s="1">
+        <v>6962.4466735154201</v>
+      </c>
+      <c r="P115" s="1">
+        <v>22847.709282207899</v>
+      </c>
+      <c r="Q115" s="1">
+        <v>12041.462082603501</v>
+      </c>
+      <c r="R115" s="1">
+        <v>11964.739364721199</v>
+      </c>
+      <c r="S115" s="1">
+        <v>50988.886645640698</v>
+      </c>
+      <c r="T115" s="1">
+        <v>4859.5221416383201</v>
+      </c>
+      <c r="U115" s="1">
+        <v>22551.168002910599</v>
+      </c>
+      <c r="V115" s="1">
+        <v>24387.425462612598</v>
+      </c>
+      <c r="W115" s="1">
+        <v>6550.6327494221796</v>
+      </c>
+      <c r="X115" s="1">
+        <v>11337.6326819818</v>
+      </c>
+      <c r="Y115" s="1">
+        <v>67380.623609226095</v>
+      </c>
+      <c r="Z115" s="1">
+        <v>2964.7800629128501</v>
+      </c>
+      <c r="AA115" s="1">
+        <v>9668.6686242915803</v>
+      </c>
+      <c r="AB115" s="1">
+        <v>27640.8794651188</v>
+      </c>
+      <c r="AC115" s="1">
+        <v>15485.410030494</v>
+      </c>
+      <c r="AD115" s="1">
+        <v>82503.322086518499</v>
+      </c>
+      <c r="AE115" s="1">
+        <v>4551.6525481538401</v>
+      </c>
+      <c r="AF115" s="1">
+        <v>18958.7600724404</v>
+      </c>
+      <c r="AG115" s="1">
+        <v>43439.351353722501</v>
+      </c>
+      <c r="AH115" s="1">
+        <v>41351.2915651168</v>
+      </c>
+      <c r="AI115" s="1">
+        <v>68781.632179178094</v>
+      </c>
+      <c r="AJ115" s="1">
+        <v>12891.599041383301</v>
+      </c>
+      <c r="AK115" s="1">
+        <v>10418.422305919799</v>
+      </c>
+      <c r="AL115" s="1">
+        <v>41111.395093067003</v>
+      </c>
+      <c r="AM115" s="1">
+        <v>295204.843584791</v>
+      </c>
+      <c r="AN115" s="1">
+        <v>39750.801511792997</v>
+      </c>
+      <c r="AO115" s="1">
+        <v>27567.566134930101</v>
+      </c>
+      <c r="AP115" s="1">
+        <v>14572.953714728001</v>
+      </c>
+      <c r="AQ115" s="1">
+        <v>19145.3598499287</v>
+      </c>
+      <c r="AR115" s="1">
+        <v>105140.230526118</v>
+      </c>
+      <c r="AS115" s="1">
+        <v>75283.359637236106</v>
+      </c>
+      <c r="AT115" s="1">
+        <v>12772.4219067919</v>
+      </c>
+      <c r="AU115" s="1">
+        <v>48041.138839253799</v>
+      </c>
+      <c r="AV115" s="1">
+        <v>19802.631173387199</v>
+      </c>
+      <c r="AW115" s="1">
+        <v>3318.4561794408901</v>
+      </c>
+      <c r="AX115" s="1">
+        <v>88911.332809744403</v>
+      </c>
+      <c r="AY115" s="1">
+        <v>13946.449861724101</v>
+      </c>
+      <c r="AZ115" s="1">
+        <v>42764.494403235301</v>
+      </c>
+      <c r="BA115" s="1">
+        <f t="shared" si="2"/>
+        <v>50521.135061377237</v>
+      </c>
+      <c r="BB115" s="1">
+        <f t="shared" si="3"/>
+        <v>76027.610496218986</v>
+      </c>
+    </row>
+    <row r="116" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A116" s="2"/>
+      <c r="B116" t="s">
+        <v>59</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1.0436108929882</v>
+      </c>
+      <c r="D116" s="1">
+        <v>1.72638028718065</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0.83987656558698298</v>
+      </c>
+      <c r="F116" s="1">
+        <v>4.1510203774680603</v>
+      </c>
+      <c r="G116" s="1">
+        <v>1.0198708327776</v>
+      </c>
+      <c r="H116" s="1">
+        <v>2.8381976294073099</v>
+      </c>
+      <c r="I116" s="1">
+        <v>7.1817897291965798</v>
+      </c>
+      <c r="J116" s="1">
+        <v>1.85745054173478</v>
+      </c>
+      <c r="K116" s="1">
+        <v>5.2796945220447897</v>
+      </c>
+      <c r="L116" s="1">
+        <v>1.35437766220293</v>
+      </c>
+      <c r="M116" s="1">
+        <v>0.46561021121117202</v>
+      </c>
+      <c r="N116" s="1">
+        <v>0.81687487308531104</v>
+      </c>
+      <c r="O116" s="1">
+        <v>1.47521511696865</v>
+      </c>
+      <c r="P116" s="1">
+        <v>5.9382268100797804</v>
+      </c>
+      <c r="Q116" s="1">
+        <v>2.74927967949237</v>
+      </c>
+      <c r="R116" s="1">
+        <v>1.1412009445721401</v>
+      </c>
+      <c r="S116" s="1">
+        <v>1.10246973608724</v>
+      </c>
+      <c r="T116" s="1">
+        <v>1.47639600720555</v>
+      </c>
+      <c r="U116" s="1">
+        <v>1.8219412013952101</v>
+      </c>
+      <c r="V116" s="1">
+        <v>2.2568305846425498</v>
+      </c>
+      <c r="W116" s="1">
+        <v>1.2196034263598901</v>
+      </c>
+      <c r="X116" s="1">
+        <v>0.62003992058247204</v>
+      </c>
+      <c r="Y116" s="1">
+        <v>0.40325630154502201</v>
+      </c>
+      <c r="Z116" s="1">
+        <v>0.38995595367973801</v>
+      </c>
+      <c r="AA116" s="1">
+        <v>0.46165996981330398</v>
+      </c>
+      <c r="AB116" s="1">
+        <v>2.3198537723817099</v>
+      </c>
+      <c r="AC116" s="1">
+        <v>0.72009238606689796</v>
+      </c>
+      <c r="AD116" s="1">
+        <v>1.3831296071501</v>
+      </c>
+      <c r="AE116" s="1">
+        <v>1.2602076916832501</v>
+      </c>
+      <c r="AF116" s="1">
+        <v>1.23391655727488</v>
+      </c>
+      <c r="AG116" s="1">
+        <v>5.0714405599408998</v>
+      </c>
+      <c r="AH116" s="1">
+        <v>1.54204980387825</v>
+      </c>
+      <c r="AI116" s="1">
+        <v>1.1008760208755599</v>
+      </c>
+      <c r="AJ116" s="1">
+        <v>1.3900861082973599</v>
+      </c>
+      <c r="AK116" s="1">
+        <v>2.1745824900319599</v>
+      </c>
+      <c r="AL116" s="1">
+        <v>11.741987506459999</v>
+      </c>
+      <c r="AM116" s="1">
+        <v>5.4756731302224004</v>
+      </c>
+      <c r="AN116" s="1">
+        <v>0.53909577325849001</v>
+      </c>
+      <c r="AO116" s="1">
+        <v>0.99160560686815402</v>
+      </c>
+      <c r="AP116" s="1">
+        <v>1.35493541690843</v>
+      </c>
+      <c r="AQ116" s="1">
+        <v>0.90310072716254397</v>
+      </c>
+      <c r="AR116" s="1">
+        <v>0.86578735733938805</v>
+      </c>
+      <c r="AS116" s="1">
+        <v>0.78999162299098902</v>
+      </c>
+      <c r="AT116" s="1">
+        <v>5.1727499776527397</v>
+      </c>
+      <c r="AU116" s="1">
+        <v>1.01374926402481</v>
+      </c>
+      <c r="AV116" s="1">
+        <v>1.0027725904196201</v>
+      </c>
+      <c r="AW116" s="1">
+        <v>6.6583583714709</v>
+      </c>
+      <c r="AX116" s="1">
+        <v>2.4203634293648402</v>
+      </c>
+      <c r="AY116" s="1">
+        <v>0.25103699334407897</v>
+      </c>
+      <c r="AZ116" s="1">
+        <v>2.4452964702083699</v>
+      </c>
+      <c r="BA116" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1890713802516979</v>
+      </c>
+      <c r="BB116" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2032002464218823</v>
+      </c>
+    </row>
+    <row r="117" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A117" s="2"/>
+      <c r="B117" t="s">
+        <v>60</v>
+      </c>
+      <c r="C117" s="1">
+        <v>5.8249836253585297E-7</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1.7217810860325598E-5</v>
+      </c>
+      <c r="E117" s="1">
+        <v>6.9450286316183804E-9</v>
+      </c>
+      <c r="F117" s="1">
+        <v>7.8551672586357408E-6</v>
+      </c>
+      <c r="G117" s="1">
+        <v>7.9967412043239794E-5</v>
+      </c>
+      <c r="H117" s="1">
+        <v>1.51120971987583E-6</v>
+      </c>
+      <c r="I117" s="1">
+        <v>9.4341813709211401E-6</v>
+      </c>
+      <c r="J117" s="1">
+        <v>2.0576353045272202E-6</v>
+      </c>
+      <c r="K117" s="1">
+        <v>2.10941486595825E-7</v>
+      </c>
+      <c r="L117" s="1">
+        <v>2.14667484556671E-5</v>
+      </c>
+      <c r="M117" s="1">
+        <v>3.2806903397412999E-6</v>
+      </c>
+      <c r="N117" s="1">
+        <v>1.7412452560937502E-5</v>
+      </c>
+      <c r="O117" s="1">
+        <v>7.52415532550057E-8</v>
+      </c>
+      <c r="P117" s="1">
+        <v>7.9827756734575301E-6</v>
+      </c>
+      <c r="Q117" s="1">
+        <v>5.6588792821873901E-6</v>
+      </c>
+      <c r="R117" s="1">
+        <v>1.49582378116441E-5</v>
+      </c>
+      <c r="S117" s="1">
+        <v>4.6390062113503898E-8</v>
+      </c>
+      <c r="T117" s="1">
+        <v>8.2748147733360906E-5</v>
+      </c>
+      <c r="U117" s="1">
+        <v>2.2119897165550799E-6</v>
+      </c>
+      <c r="V117" s="1">
+        <v>3.3377382222281802E-5</v>
+      </c>
+      <c r="W117" s="1">
+        <v>5.0424801342223099E-4</v>
+      </c>
+      <c r="X117" s="1">
+        <v>1.6819654895497301E-5</v>
+      </c>
+      <c r="Y117" s="1">
+        <v>1.9590786268939101E-5</v>
+      </c>
+      <c r="Z117" s="1">
+        <v>3.5742604111450898E-4</v>
+      </c>
+      <c r="AA117" s="1">
+        <v>1.67984497387461E-6</v>
+      </c>
+      <c r="AB117" s="1">
+        <v>8.7332532482256696E-7</v>
+      </c>
+      <c r="AC117" s="1">
+        <v>4.28005592704654E-6</v>
+      </c>
+      <c r="AD117" s="1">
+        <v>2.1515326345874999E-5</v>
+      </c>
+      <c r="AE117" s="1">
+        <v>2.1430278927242399E-6</v>
+      </c>
+      <c r="AF117" s="1">
+        <v>3.32912334944149E-6</v>
+      </c>
+      <c r="AG117" s="1">
+        <v>2.5725801687245602E-4</v>
+      </c>
+      <c r="AH117" s="1">
+        <v>2.4792066867375902E-6</v>
+      </c>
+      <c r="AI117" s="1">
+        <v>2.9929501973499602E-6</v>
+      </c>
+      <c r="AJ117" s="1">
+        <v>2.1102377129727999E-5</v>
+      </c>
+      <c r="AK117" s="1">
+        <v>1.9645003953325899E-7</v>
+      </c>
+      <c r="AL117" s="1">
+        <v>2.6008508362792599E-8</v>
+      </c>
+      <c r="AM117" s="1">
+        <v>2.5214670887819401E-6</v>
+      </c>
+      <c r="AN117" s="1">
+        <v>2.43397130404197E-5</v>
+      </c>
+      <c r="AO117" s="1">
+        <v>5.8976323018190303E-6</v>
+      </c>
+      <c r="AP117" s="1">
+        <v>3.4695401408796699E-6</v>
+      </c>
+      <c r="AQ117" s="1">
+        <v>2.7307972479456E-4</v>
+      </c>
+      <c r="AR117" s="1">
+        <v>3.3396440608127603E-5</v>
+      </c>
+      <c r="AS117" s="1">
+        <v>3.0736061004766497E-5</v>
+      </c>
+      <c r="AT117" s="1">
+        <v>1.4376477732654E-5</v>
+      </c>
+      <c r="AU117" s="1">
+        <v>4.2992755528008297E-6</v>
+      </c>
+      <c r="AV117" s="1">
+        <v>2.6167020752087401E-5</v>
+      </c>
+      <c r="AW117" s="1">
+        <v>1.43134744321773E-6</v>
+      </c>
+      <c r="AX117" s="1">
+        <v>5.1026152619875501E-7</v>
+      </c>
+      <c r="AY117" s="1">
+        <v>1.6143329607926101E-8</v>
+      </c>
+      <c r="AZ117" s="1">
+        <v>1.31463419836148E-6</v>
+      </c>
+      <c r="BA117" s="1">
+        <f t="shared" si="2"/>
+        <v>3.8911573706198E-5</v>
+      </c>
+      <c r="BB117" s="1">
+        <f t="shared" si="3"/>
+        <v>9.6770309962895706E-5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+      <c r="N118" s="1"/>
+      <c r="O118" s="1"/>
+      <c r="P118" s="1"/>
+      <c r="Q118" s="1"/>
+      <c r="R118" s="1"/>
+      <c r="S118" s="1"/>
+      <c r="T118" s="1"/>
+      <c r="U118" s="1"/>
+      <c r="V118" s="1"/>
+      <c r="W118" s="1"/>
+      <c r="X118" s="1"/>
+      <c r="Y118" s="1"/>
+      <c r="Z118" s="1"/>
+      <c r="AA118" s="1"/>
+      <c r="AB118" s="1"/>
+      <c r="AC118" s="1"/>
+      <c r="AD118" s="1"/>
+      <c r="AE118" s="1"/>
+      <c r="AF118" s="1"/>
+      <c r="AG118" s="1"/>
+      <c r="AH118" s="1"/>
+      <c r="AI118" s="1"/>
+      <c r="AJ118" s="1"/>
+      <c r="AK118" s="1"/>
+      <c r="AL118" s="1"/>
+      <c r="AM118" s="1"/>
+      <c r="AN118" s="1"/>
+      <c r="AO118" s="1"/>
+      <c r="AP118" s="1"/>
+      <c r="AQ118" s="1"/>
+      <c r="AR118" s="1"/>
+      <c r="AS118" s="1"/>
+      <c r="AT118" s="1"/>
+      <c r="AU118" s="1"/>
+      <c r="AV118" s="1"/>
+      <c r="AW118" s="1"/>
+      <c r="AX118" s="1"/>
+      <c r="AY118" s="1"/>
+      <c r="AZ118" s="1"/>
+      <c r="BA118" s="1"/>
+      <c r="BB118" s="1"/>
+    </row>
+    <row r="119" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B119" t="s">
+        <v>53</v>
+      </c>
+      <c r="C119" s="1">
+        <v>13.725063115504801</v>
+      </c>
+      <c r="D119" s="1">
+        <v>14.929610272474999</v>
+      </c>
+      <c r="E119" s="1">
+        <v>14.2022396323202</v>
+      </c>
+      <c r="F119" s="1">
+        <v>13.246007239177199</v>
+      </c>
+      <c r="G119" s="1">
+        <v>13.741949215148599</v>
+      </c>
+      <c r="H119" s="1">
+        <v>14.1353448295901</v>
+      </c>
+      <c r="I119" s="1">
+        <v>13.713395523946</v>
+      </c>
+      <c r="J119" s="1">
+        <v>14.8385838106738</v>
+      </c>
+      <c r="K119" s="1">
+        <v>15.293203815758201</v>
+      </c>
+      <c r="L119" s="1">
+        <v>15.3885209000068</v>
+      </c>
+      <c r="M119" s="1">
+        <v>14.2363139005652</v>
+      </c>
+      <c r="N119" s="1">
+        <v>13.498361942714199</v>
+      </c>
+      <c r="O119" s="1">
+        <v>12.9645955500987</v>
+      </c>
+      <c r="P119" s="1">
+        <v>14.512076738415599</v>
+      </c>
+      <c r="Q119" s="1">
+        <v>13.3577682182753</v>
+      </c>
+      <c r="R119" s="1">
+        <v>14.5355165151598</v>
+      </c>
+      <c r="S119" s="1">
+        <v>11.6239765638812</v>
+      </c>
+      <c r="T119" s="1">
+        <v>13.4113805100699</v>
+      </c>
+      <c r="U119" s="1">
+        <v>13.913951627155001</v>
+      </c>
+      <c r="V119" s="1">
+        <v>13.491477191127199</v>
+      </c>
+      <c r="W119" s="1">
+        <v>14.5322429464262</v>
+      </c>
+      <c r="X119" s="1">
+        <v>13.252012104393099</v>
+      </c>
+      <c r="Y119" s="1">
+        <v>14.0962087293916</v>
+      </c>
+      <c r="Z119" s="1">
+        <v>14.1474896296618</v>
+      </c>
+      <c r="AA119" s="1">
+        <v>14.213833366698699</v>
+      </c>
+      <c r="AB119" s="1">
+        <v>14.7918086430965</v>
+      </c>
+      <c r="AC119" s="1">
+        <v>14.905531034528201</v>
+      </c>
+      <c r="AD119" s="1">
+        <v>14.5756361316579</v>
+      </c>
+      <c r="AE119" s="1">
+        <v>12.200499376005499</v>
+      </c>
+      <c r="AF119" s="1">
+        <v>13.8703553217955</v>
+      </c>
+      <c r="AG119" s="1">
+        <v>14.6737471427607</v>
+      </c>
+      <c r="AH119" s="1">
+        <v>11.9449418632292</v>
+      </c>
+      <c r="AI119" s="1">
+        <v>15.1456792795683</v>
+      </c>
+      <c r="AJ119" s="1">
+        <v>12.5502232841542</v>
+      </c>
+      <c r="AK119" s="1">
+        <v>15.0173119817669</v>
+      </c>
+      <c r="AL119" s="1">
+        <v>14.385313705003499</v>
+      </c>
+      <c r="AM119" s="1">
+        <v>12.510323582684499</v>
+      </c>
+      <c r="AN119" s="1">
+        <v>14.010123193043199</v>
+      </c>
+      <c r="AO119" s="1">
+        <v>14.4184088515587</v>
+      </c>
+      <c r="AP119" s="1">
+        <v>10.9052135360336</v>
+      </c>
+      <c r="AQ119" s="1">
+        <v>13.6182238986821</v>
+      </c>
+      <c r="AR119" s="1">
+        <v>14.3380266479488</v>
+      </c>
+      <c r="AS119" s="1">
+        <v>15.9096702829703</v>
+      </c>
+      <c r="AT119" s="1">
+        <v>12.8943544674535</v>
+      </c>
+      <c r="AU119" s="1">
+        <v>14.641872971054299</v>
+      </c>
+      <c r="AV119" s="1">
+        <v>15.954923596471399</v>
+      </c>
+      <c r="AW119" s="1">
+        <v>14.9379794565409</v>
+      </c>
+      <c r="AX119" s="1">
+        <v>14.655840043246</v>
+      </c>
+      <c r="AY119" s="1">
+        <v>14.3754618326267</v>
+      </c>
+      <c r="AZ119" s="1">
+        <v>13.704301704095</v>
+      </c>
+      <c r="BA119" s="1">
+        <f t="shared" si="2"/>
+        <v>13.998737914332194</v>
+      </c>
+      <c r="BB119" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0268390752579877</v>
+      </c>
+    </row>
+    <row r="120" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A120" s="2"/>
+      <c r="B120" t="s">
+        <v>54</v>
+      </c>
+      <c r="C120" s="1">
+        <v>112.57202337642001</v>
+      </c>
+      <c r="D120" s="1">
+        <v>122.245250771849</v>
+      </c>
+      <c r="E120" s="1">
+        <v>114.260706167047</v>
+      </c>
+      <c r="F120" s="1">
+        <v>143.439791317117</v>
+      </c>
+      <c r="G120" s="1">
+        <v>117.677146419596</v>
+      </c>
+      <c r="H120" s="1">
+        <v>131.93205175894701</v>
+      </c>
+      <c r="I120" s="1">
+        <v>136.31512691645301</v>
+      </c>
+      <c r="J120" s="1">
+        <v>109.728905560092</v>
+      </c>
+      <c r="K120" s="1">
+        <v>143.47229242807001</v>
+      </c>
+      <c r="L120" s="1">
+        <v>124.920427392861</v>
+      </c>
+      <c r="M120" s="1">
+        <v>112.134927219231</v>
+      </c>
+      <c r="N120" s="1">
+        <v>121.374002683215</v>
+      </c>
+      <c r="O120" s="1">
+        <v>135.054795263702</v>
+      </c>
+      <c r="P120" s="1">
+        <v>121.096756050514</v>
+      </c>
+      <c r="Q120" s="1">
+        <v>125.454794527921</v>
+      </c>
+      <c r="R120" s="1">
+        <v>133.040190779553</v>
+      </c>
+      <c r="S120" s="1">
+        <v>136.991842195228</v>
+      </c>
+      <c r="T120" s="1">
+        <v>124.144135171004</v>
+      </c>
+      <c r="U120" s="1">
+        <v>113.159628347048</v>
+      </c>
+      <c r="V120" s="1">
+        <v>111.79940701045</v>
+      </c>
+      <c r="W120" s="1">
+        <v>143.18795456099599</v>
+      </c>
+      <c r="X120" s="1">
+        <v>119.877469473316</v>
+      </c>
+      <c r="Y120" s="1">
+        <v>113.163127639319</v>
+      </c>
+      <c r="Z120" s="1">
+        <v>139.47327132316701</v>
+      </c>
+      <c r="AA120" s="1">
+        <v>106.524652464363</v>
+      </c>
+      <c r="AB120" s="1">
+        <v>126.779532052919</v>
+      </c>
+      <c r="AC120" s="1">
+        <v>92.146213036891297</v>
+      </c>
+      <c r="AD120" s="1">
+        <v>129.42307514928001</v>
+      </c>
+      <c r="AE120" s="1">
+        <v>127.37765051778</v>
+      </c>
+      <c r="AF120" s="1">
+        <v>132.005577128429</v>
+      </c>
+      <c r="AG120" s="1">
+        <v>120.434673203038</v>
+      </c>
+      <c r="AH120" s="1">
+        <v>142.79445507002799</v>
+      </c>
+      <c r="AI120" s="1">
+        <v>162.08395971614701</v>
+      </c>
+      <c r="AJ120" s="1">
+        <v>118.912633711636</v>
+      </c>
+      <c r="AK120" s="1">
+        <v>112.983371634215</v>
+      </c>
+      <c r="AL120" s="1">
+        <v>90.176105183252403</v>
+      </c>
+      <c r="AM120" s="1">
+        <v>142.80637325126699</v>
+      </c>
+      <c r="AN120" s="1">
+        <v>130.697385635915</v>
+      </c>
+      <c r="AO120" s="1">
+        <v>120.94290903487099</v>
+      </c>
+      <c r="AP120" s="1">
+        <v>124.14655437371999</v>
+      </c>
+      <c r="AQ120" s="1">
+        <v>128.58656595154201</v>
+      </c>
+      <c r="AR120" s="1">
+        <v>117.442930843702</v>
+      </c>
+      <c r="AS120" s="1">
+        <v>93.750534864580302</v>
+      </c>
+      <c r="AT120" s="1">
+        <v>120.189907880646</v>
+      </c>
+      <c r="AU120" s="1">
+        <v>101.023695092571</v>
+      </c>
+      <c r="AV120" s="1">
+        <v>109.175101677057</v>
+      </c>
+      <c r="AW120" s="1">
+        <v>149.17514126201399</v>
+      </c>
+      <c r="AX120" s="1">
+        <v>116.243788743983</v>
+      </c>
+      <c r="AY120" s="1">
+        <v>135.754426948419</v>
+      </c>
+      <c r="AZ120" s="1">
+        <v>101.341401782487</v>
+      </c>
+      <c r="BA120" s="1">
+        <f t="shared" si="2"/>
+        <v>123.18869281127739</v>
+      </c>
+      <c r="BB120" s="1">
+        <f t="shared" si="3"/>
+        <v>14.823051893884768</v>
+      </c>
+    </row>
+    <row r="121" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A121" s="2"/>
+      <c r="B121" t="s">
+        <v>55</v>
+      </c>
+      <c r="C121" s="1">
+        <v>56.010657151461601</v>
+      </c>
+      <c r="D121" s="1">
+        <v>36.962175094588801</v>
+      </c>
+      <c r="E121" s="1">
+        <v>46.519023343913602</v>
+      </c>
+      <c r="F121" s="1">
+        <v>47.408494147859699</v>
+      </c>
+      <c r="G121" s="1">
+        <v>46.419714039845097</v>
+      </c>
+      <c r="H121" s="1">
+        <v>49.577518193308798</v>
+      </c>
+      <c r="I121" s="1">
+        <v>40.276744376453301</v>
+      </c>
+      <c r="J121" s="1">
+        <v>49.6109602838306</v>
+      </c>
+      <c r="K121" s="1">
+        <v>43.349396952215599</v>
+      </c>
+      <c r="L121" s="1">
+        <v>53.245861528625298</v>
+      </c>
+      <c r="M121" s="1">
+        <v>41.922414874748299</v>
+      </c>
+      <c r="N121" s="1">
+        <v>49.563429096629498</v>
+      </c>
+      <c r="O121" s="1">
+        <v>33.501683897391203</v>
+      </c>
+      <c r="P121" s="1">
+        <v>35.296160576412603</v>
+      </c>
+      <c r="Q121" s="1">
+        <v>33.363986984422503</v>
+      </c>
+      <c r="R121" s="1">
+        <v>58.5884932420159</v>
+      </c>
+      <c r="S121" s="1">
+        <v>33.937615071540399</v>
+      </c>
+      <c r="T121" s="1">
+        <v>47.204489905653098</v>
+      </c>
+      <c r="U121" s="1">
+        <v>36.629537399538201</v>
+      </c>
+      <c r="V121" s="1">
+        <v>49.431237774036603</v>
+      </c>
+      <c r="W121" s="1">
+        <v>51.745834283618599</v>
+      </c>
+      <c r="X121" s="1">
+        <v>62.725487267326699</v>
+      </c>
+      <c r="Y121" s="1">
+        <v>36.189692791470797</v>
+      </c>
+      <c r="Z121" s="1">
+        <v>43.888577055600599</v>
+      </c>
+      <c r="AA121" s="1">
+        <v>47.464987643277901</v>
+      </c>
+      <c r="AB121" s="1">
+        <v>42.429007583257103</v>
+      </c>
+      <c r="AC121" s="1">
+        <v>37.620743197590897</v>
+      </c>
+      <c r="AD121" s="1">
+        <v>44.707624521294299</v>
+      </c>
+      <c r="AE121" s="1">
+        <v>65.391805473369701</v>
+      </c>
+      <c r="AF121" s="1">
+        <v>50.682437094504103</v>
+      </c>
+      <c r="AG121" s="1">
+        <v>42.3573403420299</v>
+      </c>
+      <c r="AH121" s="1">
+        <v>35.266800191128603</v>
+      </c>
+      <c r="AI121" s="1">
+        <v>43.069996187040701</v>
+      </c>
+      <c r="AJ121" s="1">
+        <v>45.269539606036197</v>
+      </c>
+      <c r="AK121" s="1">
+        <v>48.5639647347002</v>
+      </c>
+      <c r="AL121" s="1">
+        <v>44.678914324934603</v>
+      </c>
+      <c r="AM121" s="1">
+        <v>42.701634346434602</v>
+      </c>
+      <c r="AN121" s="1">
+        <v>46.357984684314999</v>
+      </c>
+      <c r="AO121" s="1">
+        <v>48.675730529333798</v>
+      </c>
+      <c r="AP121" s="1">
+        <v>24.913694537886801</v>
+      </c>
+      <c r="AQ121" s="1">
+        <v>58.124340656947801</v>
+      </c>
+      <c r="AR121" s="1">
+        <v>53.442522386736997</v>
+      </c>
+      <c r="AS121" s="1">
+        <v>53.393969236964601</v>
+      </c>
+      <c r="AT121" s="1">
+        <v>58.376349293924797</v>
+      </c>
+      <c r="AU121" s="1">
+        <v>37.097911938808899</v>
+      </c>
+      <c r="AV121" s="1">
+        <v>47.474270591824201</v>
+      </c>
+      <c r="AW121" s="1">
+        <v>45.839169313993501</v>
+      </c>
+      <c r="AX121" s="1">
+        <v>50.072316299301498</v>
+      </c>
+      <c r="AY121" s="1">
+        <v>45.501177143748002</v>
+      </c>
+      <c r="AZ121" s="1">
+        <v>39.403071247161698</v>
+      </c>
+      <c r="BA121" s="1">
+        <f t="shared" si="2"/>
+        <v>45.644929768781068</v>
+      </c>
+      <c r="BB121" s="1">
+        <f t="shared" si="3"/>
+        <v>8.0247908659515925</v>
+      </c>
+    </row>
+    <row r="122" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A122" s="2"/>
+      <c r="B122" t="s">
+        <v>56</v>
+      </c>
+      <c r="C122" s="1">
+        <v>9.7127301907187995</v>
+      </c>
+      <c r="D122" s="1">
+        <v>10.390694203400599</v>
+      </c>
+      <c r="E122" s="1">
+        <v>10.0945100603527</v>
+      </c>
+      <c r="F122" s="1">
+        <v>9.7472705468419392</v>
+      </c>
+      <c r="G122" s="1">
+        <v>9.9210427832773007</v>
+      </c>
+      <c r="H122" s="1">
+        <v>11.5528553839992</v>
+      </c>
+      <c r="I122" s="1">
+        <v>9.5883840880325302</v>
+      </c>
+      <c r="J122" s="1">
+        <v>7.5037286364990701</v>
+      </c>
+      <c r="K122" s="1">
+        <v>8.4458831054014407</v>
+      </c>
+      <c r="L122" s="1">
+        <v>8.0634967331767307</v>
+      </c>
+      <c r="M122" s="1">
+        <v>12.1409334534947</v>
+      </c>
+      <c r="N122" s="1">
+        <v>8.7280075917589706</v>
+      </c>
+      <c r="O122" s="1">
+        <v>11.936404376176901</v>
+      </c>
+      <c r="P122" s="1">
+        <v>10.820345298069601</v>
+      </c>
+      <c r="Q122" s="1">
+        <v>11.2289741477412</v>
+      </c>
+      <c r="R122" s="1">
+        <v>10.645489487608399</v>
+      </c>
+      <c r="S122" s="1">
+        <v>10.842168656039799</v>
+      </c>
+      <c r="T122" s="1">
+        <v>9.9900256045781894</v>
+      </c>
+      <c r="U122" s="1">
+        <v>8.7903707277681704</v>
+      </c>
+      <c r="V122" s="1">
+        <v>10.3514897163156</v>
+      </c>
+      <c r="W122" s="1">
+        <v>10.5378002584713</v>
+      </c>
+      <c r="X122" s="1">
+        <v>7.98227234636445</v>
+      </c>
+      <c r="Y122" s="1">
+        <v>12.240582929580899</v>
+      </c>
+      <c r="Z122" s="1">
+        <v>12.166842986084999</v>
+      </c>
+      <c r="AA122" s="1">
+        <v>11.7799154338562</v>
+      </c>
+      <c r="AB122" s="1">
+        <v>10.678098849956401</v>
+      </c>
+      <c r="AC122" s="1">
+        <v>9.4912172489612701</v>
+      </c>
+      <c r="AD122" s="1">
+        <v>12.238575017916601</v>
+      </c>
+      <c r="AE122" s="1">
+        <v>8.6680158367695608</v>
+      </c>
+      <c r="AF122" s="1">
+        <v>9.0059376184120001</v>
+      </c>
+      <c r="AG122" s="1">
+        <v>10.9853649428944</v>
+      </c>
+      <c r="AH122" s="1">
+        <v>9.8616146811677208</v>
+      </c>
+      <c r="AI122" s="1">
+        <v>8.1353283611186296</v>
+      </c>
+      <c r="AJ122" s="1">
+        <v>7.83447319071783</v>
+      </c>
+      <c r="AK122" s="1">
+        <v>10.165145653876699</v>
+      </c>
+      <c r="AL122" s="1">
+        <v>9.7750362396654893</v>
+      </c>
+      <c r="AM122" s="1">
+        <v>8.8887440048525299</v>
+      </c>
+      <c r="AN122" s="1">
+        <v>9.4895134921833506</v>
+      </c>
+      <c r="AO122" s="1">
+        <v>8.9390150515623592</v>
+      </c>
+      <c r="AP122" s="1">
+        <v>11.273605102982501</v>
+      </c>
+      <c r="AQ122" s="1">
+        <v>7.1302134549233296</v>
+      </c>
+      <c r="AR122" s="1">
+        <v>10.367977122990601</v>
+      </c>
+      <c r="AS122" s="1">
+        <v>10.9848486875318</v>
+      </c>
+      <c r="AT122" s="1">
+        <v>9.3341208059472294</v>
+      </c>
+      <c r="AU122" s="1">
+        <v>9.9031706166996702</v>
+      </c>
+      <c r="AV122" s="1">
+        <v>9.4214083298334703</v>
+      </c>
+      <c r="AW122" s="1">
+        <v>8.5621991612517405</v>
+      </c>
+      <c r="AX122" s="1">
+        <v>10.109106871875399</v>
+      </c>
+      <c r="AY122" s="1">
+        <v>9.2354284002701004</v>
+      </c>
+      <c r="AZ122" s="1">
+        <v>9.1653215418522596</v>
+      </c>
+      <c r="BA122" s="1">
+        <f t="shared" si="2"/>
+        <v>9.8969139806364552</v>
+      </c>
+      <c r="BB122" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2830478603149202</v>
+      </c>
+    </row>
+    <row r="123" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A123" s="2"/>
+      <c r="B123" t="s">
+        <v>57</v>
+      </c>
+      <c r="C123" s="1">
+        <v>2024.8507511820501</v>
+      </c>
+      <c r="D123" s="1">
+        <v>2223.5041690678399</v>
+      </c>
+      <c r="E123" s="1">
+        <v>2156.7095770913602</v>
+      </c>
+      <c r="F123" s="1">
+        <v>1967.00994342437</v>
+      </c>
+      <c r="G123" s="1">
+        <v>3301.49797960461</v>
+      </c>
+      <c r="H123" s="1">
+        <v>1756.9840454909499</v>
+      </c>
+      <c r="I123" s="1">
+        <v>2933.7802511109498</v>
+      </c>
+      <c r="J123" s="1">
+        <v>1868.8090412138499</v>
+      </c>
+      <c r="K123" s="1">
+        <v>2694.3465007995501</v>
+      </c>
+      <c r="L123" s="1">
+        <v>2736.4204589552901</v>
+      </c>
+      <c r="M123" s="1">
+        <v>2568.8121864947898</v>
+      </c>
+      <c r="N123" s="1">
+        <v>4088.6539883082301</v>
+      </c>
+      <c r="O123" s="1">
+        <v>1431.9746925234999</v>
+      </c>
+      <c r="P123" s="1">
+        <v>2278.7899994821701</v>
+      </c>
+      <c r="Q123" s="1">
+        <v>2865.6289814934198</v>
+      </c>
+      <c r="R123" s="1">
+        <v>1586.52099348517</v>
+      </c>
+      <c r="S123" s="1">
+        <v>2345.2630523310499</v>
+      </c>
+      <c r="T123" s="1">
+        <v>1842.90016678643</v>
+      </c>
+      <c r="U123" s="1">
+        <v>2380.0912398061</v>
+      </c>
+      <c r="V123" s="1">
+        <v>1840.7714952010299</v>
+      </c>
+      <c r="W123" s="1">
+        <v>1689.1993171624199</v>
+      </c>
+      <c r="X123" s="1">
+        <v>2980.7976864665302</v>
+      </c>
+      <c r="Y123" s="1">
+        <v>2263.9133976426201</v>
+      </c>
+      <c r="Z123" s="1">
+        <v>2137.3487806421099</v>
+      </c>
+      <c r="AA123" s="1">
+        <v>2889.6926453744099</v>
+      </c>
+      <c r="AB123" s="1">
+        <v>1967.36937348832</v>
+      </c>
+      <c r="AC123" s="1">
+        <v>3059.1654335212102</v>
+      </c>
+      <c r="AD123" s="1">
+        <v>1970.08248353558</v>
+      </c>
+      <c r="AE123" s="1">
+        <v>2966.41690987938</v>
+      </c>
+      <c r="AF123" s="1">
+        <v>2492.71606180655</v>
+      </c>
+      <c r="AG123" s="1">
+        <v>3060.6037106714398</v>
+      </c>
+      <c r="AH123" s="1">
+        <v>2332.1704565178202</v>
+      </c>
+      <c r="AI123" s="1">
+        <v>2577.9951719871301</v>
+      </c>
+      <c r="AJ123" s="1">
+        <v>1870.87842429387</v>
+      </c>
+      <c r="AK123" s="1">
+        <v>2821.8889725026702</v>
+      </c>
+      <c r="AL123" s="1">
+        <v>3732.95645997666</v>
+      </c>
+      <c r="AM123" s="1">
+        <v>2027.8309949925001</v>
+      </c>
+      <c r="AN123" s="1">
+        <v>1814.12231553109</v>
+      </c>
+      <c r="AO123" s="1">
+        <v>2986.6630696888501</v>
+      </c>
+      <c r="AP123" s="1">
+        <v>2298.9991419105299</v>
+      </c>
+      <c r="AQ123" s="1">
+        <v>1825.1519086380899</v>
+      </c>
+      <c r="AR123" s="1">
+        <v>2303.6465945221198</v>
+      </c>
+      <c r="AS123" s="1">
+        <v>3237.3817732522698</v>
+      </c>
+      <c r="AT123" s="1">
+        <v>2635.0298922921602</v>
+      </c>
+      <c r="AU123" s="1">
+        <v>2490.7738251527098</v>
+      </c>
+      <c r="AV123" s="1">
+        <v>2286.1859005548699</v>
+      </c>
+      <c r="AW123" s="1">
+        <v>1800.96600983699</v>
+      </c>
+      <c r="AX123" s="1">
+        <v>4847.0807136366402</v>
+      </c>
+      <c r="AY123" s="1">
+        <v>1836.7842649586701</v>
+      </c>
+      <c r="AZ123" s="1">
+        <v>1839.04672432089</v>
+      </c>
+      <c r="BA123" s="1">
+        <f t="shared" si="2"/>
+        <v>2438.7235585721955</v>
+      </c>
+      <c r="BB123" s="1">
+        <f t="shared" si="3"/>
+        <v>657.5584877113904</v>
+      </c>
+    </row>
+    <row r="124" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A124" s="2"/>
+      <c r="B124" t="s">
+        <v>58</v>
+      </c>
+      <c r="C124" s="1">
+        <v>1272962.6381266201</v>
+      </c>
+      <c r="D124" s="1">
+        <v>793719.67935337406</v>
+      </c>
+      <c r="E124" s="1">
+        <v>897780.60829760996</v>
+      </c>
+      <c r="F124" s="1">
+        <v>1358236.2590793299</v>
+      </c>
+      <c r="G124" s="1">
+        <v>859252.10022891196</v>
+      </c>
+      <c r="H124" s="1">
+        <v>636753.31740623806</v>
+      </c>
+      <c r="I124" s="1">
+        <v>1499912.02492915</v>
+      </c>
+      <c r="J124" s="1">
+        <v>839069.10795207601</v>
+      </c>
+      <c r="K124" s="1">
+        <v>1186259.21899596</v>
+      </c>
+      <c r="L124" s="1">
+        <v>729551.38835715898</v>
+      </c>
+      <c r="M124" s="1">
+        <v>1086939.22350327</v>
+      </c>
+      <c r="N124" s="1">
+        <v>2875791.7355052</v>
+      </c>
+      <c r="O124" s="1">
+        <v>1121612.4294046599</v>
+      </c>
+      <c r="P124" s="1">
+        <v>1084224.12411662</v>
+      </c>
+      <c r="Q124" s="1">
+        <v>1695055.81467676</v>
+      </c>
+      <c r="R124" s="1">
+        <v>1373119.42012382</v>
+      </c>
+      <c r="S124" s="1">
+        <v>761079.60991727305</v>
+      </c>
+      <c r="T124" s="1">
+        <v>1156125.2819899099</v>
+      </c>
+      <c r="U124" s="1">
+        <v>2481131.8592276699</v>
+      </c>
+      <c r="V124" s="1">
+        <v>1175595.6120672601</v>
+      </c>
+      <c r="W124" s="1">
+        <v>947886.49084212305</v>
+      </c>
+      <c r="X124" s="1">
+        <v>1188208.54595919</v>
+      </c>
+      <c r="Y124" s="1">
+        <v>1129315.1463216001</v>
+      </c>
+      <c r="Z124" s="1">
+        <v>876310.50326252903</v>
+      </c>
+      <c r="AA124" s="1">
+        <v>577270.81877361203</v>
+      </c>
+      <c r="AB124" s="1">
+        <v>1340513.8387768201</v>
+      </c>
+      <c r="AC124" s="1">
+        <v>1766961.2466166299</v>
+      </c>
+      <c r="AD124" s="1">
+        <v>850194.00551543594</v>
+      </c>
+      <c r="AE124" s="1">
+        <v>1110905.7966159999</v>
+      </c>
+      <c r="AF124" s="1">
+        <v>1855432.2322944701</v>
+      </c>
+      <c r="AG124" s="1">
+        <v>531816.35893544497</v>
+      </c>
+      <c r="AH124" s="1">
+        <v>863442.79740536097</v>
+      </c>
+      <c r="AI124" s="1">
+        <v>1968172.4800602801</v>
+      </c>
+      <c r="AJ124" s="1">
+        <v>1810477.4269348299</v>
+      </c>
+      <c r="AK124" s="1">
+        <v>890774.51621079398</v>
+      </c>
+      <c r="AL124" s="1">
+        <v>944298.07529414794</v>
+      </c>
+      <c r="AM124" s="1">
+        <v>2414101.2347007901</v>
+      </c>
+      <c r="AN124" s="1">
+        <v>1073958.3515662299</v>
+      </c>
+      <c r="AO124" s="1">
+        <v>612632.58823327196</v>
+      </c>
+      <c r="AP124" s="1">
+        <v>1267225.1221079901</v>
+      </c>
+      <c r="AQ124" s="1">
+        <v>879278.07407950202</v>
+      </c>
+      <c r="AR124" s="1">
+        <v>1465112.2510957301</v>
+      </c>
+      <c r="AS124" s="1">
+        <v>946478.44344290905</v>
+      </c>
+      <c r="AT124" s="1">
+        <v>1615897.8605482699</v>
+      </c>
+      <c r="AU124" s="1">
+        <v>1051951.0589443</v>
+      </c>
+      <c r="AV124" s="1">
+        <v>754668.153704633</v>
+      </c>
+      <c r="AW124" s="1">
+        <v>962181.78516424901</v>
+      </c>
+      <c r="AX124" s="1">
+        <v>1147207.46371949</v>
+      </c>
+      <c r="AY124" s="1">
+        <v>997817.19402701897</v>
+      </c>
+      <c r="AZ124" s="1">
+        <v>1563591.64974279</v>
+      </c>
+      <c r="BA124" s="1">
+        <f t="shared" si="2"/>
+        <v>1205765.0592831061</v>
+      </c>
+      <c r="BB124" s="1">
+        <f t="shared" si="3"/>
+        <v>489094.6147654024</v>
+      </c>
+    </row>
+    <row r="125" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A125" s="2"/>
+      <c r="B125" t="s">
+        <v>59</v>
+      </c>
+      <c r="C125" s="1">
+        <v>21.5956154571636</v>
+      </c>
+      <c r="D125" s="1">
+        <v>34.081189806091402</v>
+      </c>
+      <c r="E125" s="1">
+        <v>28.171432207622299</v>
+      </c>
+      <c r="F125" s="1">
+        <v>36.471964719118702</v>
+      </c>
+      <c r="G125" s="1">
+        <v>30.111341429819198</v>
+      </c>
+      <c r="H125" s="1">
+        <v>30.293016916919498</v>
+      </c>
+      <c r="I125" s="1">
+        <v>31.039849961710001</v>
+      </c>
+      <c r="J125" s="1">
+        <v>27.9423611509959</v>
+      </c>
+      <c r="K125" s="1">
+        <v>31.5660300961747</v>
+      </c>
+      <c r="L125" s="1">
+        <v>26.341945714418401</v>
+      </c>
+      <c r="M125" s="1">
+        <v>32.722106467527901</v>
+      </c>
+      <c r="N125" s="1">
+        <v>26.2359348531267</v>
+      </c>
+      <c r="O125" s="1">
+        <v>24.597797456376501</v>
+      </c>
+      <c r="P125" s="1">
+        <v>35.049655078104102</v>
+      </c>
+      <c r="Q125" s="1">
+        <v>27.5582425938087</v>
+      </c>
+      <c r="R125" s="1">
+        <v>35.645744049554899</v>
+      </c>
+      <c r="S125" s="1">
+        <v>35.136497512533097</v>
+      </c>
+      <c r="T125" s="1">
+        <v>25.131404631042901</v>
+      </c>
+      <c r="U125" s="1">
+        <v>35.476729755874899</v>
+      </c>
+      <c r="V125" s="1">
+        <v>30.401319671070901</v>
+      </c>
+      <c r="W125" s="1">
+        <v>30.451798630513402</v>
+      </c>
+      <c r="X125" s="1">
+        <v>24.146156855682101</v>
+      </c>
+      <c r="Y125" s="1">
+        <v>30.515748586055501</v>
+      </c>
+      <c r="Z125" s="1">
+        <v>26.922259172855</v>
+      </c>
+      <c r="AA125" s="1">
+        <v>20.905304063439001</v>
+      </c>
+      <c r="AB125" s="1">
+        <v>33.070702346448599</v>
+      </c>
+      <c r="AC125" s="1">
+        <v>29.368913879958999</v>
+      </c>
+      <c r="AD125" s="1">
+        <v>24.4885518690228</v>
+      </c>
+      <c r="AE125" s="1">
+        <v>32.797135753290902</v>
+      </c>
+      <c r="AF125" s="1">
+        <v>33.129889184289503</v>
+      </c>
+      <c r="AG125" s="1">
+        <v>41.109440201567303</v>
+      </c>
+      <c r="AH125" s="1">
+        <v>28.6522888368319</v>
+      </c>
+      <c r="AI125" s="1">
+        <v>36.944698545987102</v>
+      </c>
+      <c r="AJ125" s="1">
+        <v>29.2049068847992</v>
+      </c>
+      <c r="AK125" s="1">
+        <v>29.433513294151801</v>
+      </c>
+      <c r="AL125" s="1">
+        <v>31.162479103519001</v>
+      </c>
+      <c r="AM125" s="1">
+        <v>37.276547320161498</v>
+      </c>
+      <c r="AN125" s="1">
+        <v>41.290603742434399</v>
+      </c>
+      <c r="AO125" s="1">
+        <v>40.825786722839602</v>
+      </c>
+      <c r="AP125" s="1">
+        <v>29.282768575635298</v>
+      </c>
+      <c r="AQ125" s="1">
+        <v>24.448249655494902</v>
+      </c>
+      <c r="AR125" s="1">
+        <v>30.911787208049699</v>
+      </c>
+      <c r="AS125" s="1">
+        <v>33.286887314069098</v>
+      </c>
+      <c r="AT125" s="1">
+        <v>25.197066740060599</v>
+      </c>
+      <c r="AU125" s="1">
+        <v>35.957538483838</v>
+      </c>
+      <c r="AV125" s="1">
+        <v>28.4558436114241</v>
+      </c>
+      <c r="AW125" s="1">
+        <v>31.4434116437629</v>
+      </c>
+      <c r="AX125" s="1">
+        <v>28.023886075274799</v>
+      </c>
+      <c r="AY125" s="1">
+        <v>28.951731334040598</v>
+      </c>
+      <c r="AZ125" s="1">
+        <v>30.288277888977699</v>
+      </c>
+      <c r="BA125" s="1">
+        <f t="shared" si="2"/>
+        <v>30.670287061070589</v>
+      </c>
+      <c r="BB125" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6794645151704453</v>
+      </c>
+    </row>
+    <row r="126" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A126" s="2"/>
+      <c r="B126" t="s">
+        <v>60</v>
+      </c>
+      <c r="C126" s="1">
+        <v>1.29549039259584E-3</v>
+      </c>
+      <c r="D126" s="1">
+        <v>1.1105803613182699E-3</v>
+      </c>
+      <c r="E126" s="1">
+        <v>4.4451079523797E-4</v>
+      </c>
+      <c r="F126" s="1">
+        <v>6.49893681752758E-4</v>
+      </c>
+      <c r="G126" s="1">
+        <v>9.54070502694203E-4</v>
+      </c>
+      <c r="H126" s="1">
+        <v>1.6646112326731001E-3</v>
+      </c>
+      <c r="I126" s="1">
+        <v>8.7502175724417201E-4</v>
+      </c>
+      <c r="J126" s="1">
+        <v>9.0509503787991499E-4</v>
+      </c>
+      <c r="K126" s="1">
+        <v>2.5341380494715801E-3</v>
+      </c>
+      <c r="L126" s="1">
+        <v>2.1485380915534599E-3</v>
+      </c>
+      <c r="M126" s="1">
+        <v>7.7000640297780201E-4</v>
+      </c>
+      <c r="N126" s="1">
+        <v>8.2993621558472605E-4</v>
+      </c>
+      <c r="O126" s="1">
+        <v>4.6144326086785701E-4</v>
+      </c>
+      <c r="P126" s="1">
+        <v>2.5667107571432902E-3</v>
+      </c>
+      <c r="Q126" s="1">
+        <v>9.0399601762743598E-4</v>
+      </c>
+      <c r="R126" s="1">
+        <v>5.1152079476056E-5</v>
+      </c>
+      <c r="S126" s="1">
+        <v>5.1854675656486798E-4</v>
+      </c>
+      <c r="T126" s="1">
+        <v>1.3807401880576401E-3</v>
+      </c>
+      <c r="U126" s="1">
+        <v>7.2205868249895202E-4</v>
+      </c>
+      <c r="V126" s="1">
+        <v>1.24939609670123E-3</v>
+      </c>
+      <c r="W126" s="1">
+        <v>3.81497208425364E-4</v>
+      </c>
+      <c r="X126" s="1">
+        <v>2.0952520108754899E-3</v>
+      </c>
+      <c r="Y126" s="1">
+        <v>3.1348811692654099E-4</v>
+      </c>
+      <c r="Z126" s="1">
+        <v>3.8089382433486598E-4</v>
+      </c>
+      <c r="AA126" s="1">
+        <v>3.0506946737324101E-4</v>
+      </c>
+      <c r="AB126" s="1">
+        <v>2.4804332589143697E-4</v>
+      </c>
+      <c r="AC126" s="1">
+        <v>2.9363655435532098E-4</v>
+      </c>
+      <c r="AD126" s="1">
+        <v>7.6270251272878801E-4</v>
+      </c>
+      <c r="AE126" s="1">
+        <v>5.6510100252135098E-3</v>
+      </c>
+      <c r="AF126" s="1">
+        <v>2.3866785225295098E-3</v>
+      </c>
+      <c r="AG126" s="1">
+        <v>4.9626371091491001E-3</v>
+      </c>
+      <c r="AH126" s="1">
+        <v>5.3256663479894404E-4</v>
+      </c>
+      <c r="AI126" s="1">
+        <v>1.71075634087331E-3</v>
+      </c>
+      <c r="AJ126" s="1">
+        <v>4.2822958587562901E-4</v>
+      </c>
+      <c r="AK126" s="1">
+        <v>2.7193614861841298E-3</v>
+      </c>
+      <c r="AL126" s="1">
+        <v>1.02081888544776E-3</v>
+      </c>
+      <c r="AM126" s="1">
+        <v>1.1320355453731099E-3</v>
+      </c>
+      <c r="AN126" s="1">
+        <v>2.59830711239147E-3</v>
+      </c>
+      <c r="AO126" s="1">
+        <v>2.7059109802374199E-4</v>
+      </c>
+      <c r="AP126" s="1">
+        <v>1.0710910033821001E-3</v>
+      </c>
+      <c r="AQ126" s="1">
+        <v>5.0215165572893699E-5</v>
+      </c>
+      <c r="AR126" s="1">
+        <v>1.2520563262905899E-3</v>
+      </c>
+      <c r="AS126" s="1">
+        <v>3.7274453886302901E-4</v>
+      </c>
+      <c r="AT126" s="1">
+        <v>1.29546106362584E-3</v>
+      </c>
+      <c r="AU126" s="1">
+        <v>3.8065895997376397E-4</v>
+      </c>
+      <c r="AV126" s="1">
+        <v>9.5709812182810704E-4</v>
+      </c>
+      <c r="AW126" s="1">
+        <v>2.2035732427647299E-4</v>
+      </c>
+      <c r="AX126" s="1">
+        <v>2.6889730269541098E-4</v>
+      </c>
+      <c r="AY126" s="1">
+        <v>1.0041348775062099E-3</v>
+      </c>
+      <c r="AZ126" s="1">
+        <v>7.0340151403407397E-4</v>
+      </c>
+      <c r="BA126" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1561125584948176E-3</v>
+      </c>
+      <c r="BB126" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1061785958227919E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="A110:A117"/>
+    <mergeCell ref="A119:A126"/>
     <mergeCell ref="A92:A99"/>
     <mergeCell ref="A101:A108"/>
     <mergeCell ref="A2:A9"/>

</xml_diff>